<commit_message>
Updates and adding data
</commit_message>
<xml_diff>
--- a/Time Series Analysis/iShades APAC v1.1.xlsx
+++ b/Time Series Analysis/iShades APAC v1.1.xlsx
@@ -1,15 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21721"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IBM_ADMIN\Desktop\Eugene's\Time Series Analysis\Time Series Analysis\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3400" yWindow="1620" windowWidth="24720" windowHeight="17500" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15330" windowHeight="6585" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Case" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -19,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="49">
   <si>
     <t>PRODUCT DEMAND ANALYSIS - iShades</t>
   </si>
@@ -154,6 +159,18 @@
   </si>
   <si>
     <t>Question 3:  Zooming in on Japan RSLR, we have 1000 units of each colour in current inventory and we have another 3000 units available (colour yet to be defined), what mix would you build these units ?</t>
+  </si>
+  <si>
+    <t>Ratio to Pink</t>
+  </si>
+  <si>
+    <t>Ratio to Silver</t>
+  </si>
+  <si>
+    <t>Average</t>
+  </si>
+  <si>
+    <t>Overall Average</t>
   </si>
 </sst>
 </file>
@@ -166,7 +183,7 @@
     <numFmt numFmtId="165" formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* &quot;-&quot;?_);_(@_)"/>
     <numFmt numFmtId="166" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;?_);_(@_)"/>
   </numFmts>
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -279,6 +296,12 @@
       <sz val="12"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -513,7 +536,7 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="106">
+  <cellXfs count="110">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -636,18 +659,6 @@
     <xf numFmtId="164" fontId="10" fillId="3" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="10" fillId="3" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -665,6 +676,30 @@
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="17" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="22">
@@ -693,6 +728,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1018,104 +1061,107 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+  <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:Z92"/>
+  <dimension ref="A1:AB92"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="R25" sqref="R25"/>
+    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="120" workbookViewId="0">
+      <selection activeCell="V58" sqref="V58"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.1640625" customWidth="1"/>
-    <col min="2" max="2" width="18.83203125" customWidth="1"/>
-    <col min="3" max="15" width="8.6640625" customWidth="1"/>
+    <col min="1" max="1" width="19.125" customWidth="1"/>
+    <col min="2" max="2" width="18.875" customWidth="1"/>
+    <col min="3" max="15" width="8.625" customWidth="1"/>
     <col min="16" max="16" width="9" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="13.5" customWidth="1"/>
+    <col min="21" max="21" width="12.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="18">
-      <c r="A1" s="92" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="92"/>
-      <c r="C1" s="92"/>
-      <c r="D1" s="92"/>
-      <c r="E1" s="92"/>
-      <c r="F1" s="92"/>
-      <c r="G1" s="92"/>
-      <c r="H1" s="92"/>
-      <c r="I1" s="92"/>
-      <c r="J1" s="92"/>
-      <c r="K1" s="92"/>
-      <c r="L1" s="92"/>
-      <c r="M1" s="92"/>
-      <c r="N1" s="92"/>
-      <c r="O1" s="92"/>
-      <c r="P1" s="92"/>
-    </row>
-    <row r="2" spans="1:18" ht="10" customHeight="1">
-      <c r="B2" s="93"/>
-      <c r="C2" s="93"/>
-      <c r="D2" s="93"/>
-      <c r="E2" s="93"/>
-      <c r="F2" s="93"/>
-      <c r="G2" s="93"/>
-      <c r="H2" s="93"/>
-      <c r="I2" s="93"/>
-      <c r="J2" s="93"/>
-      <c r="K2" s="93"/>
-      <c r="L2" s="93"/>
-      <c r="M2" s="93"/>
-      <c r="N2" s="93"/>
-      <c r="O2" s="93"/>
-    </row>
-    <row r="3" spans="1:18">
+    <row r="1" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="102" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="102"/>
+      <c r="C1" s="102"/>
+      <c r="D1" s="102"/>
+      <c r="E1" s="102"/>
+      <c r="F1" s="102"/>
+      <c r="G1" s="102"/>
+      <c r="H1" s="102"/>
+      <c r="I1" s="102"/>
+      <c r="J1" s="102"/>
+      <c r="K1" s="102"/>
+      <c r="L1" s="102"/>
+      <c r="M1" s="102"/>
+      <c r="N1" s="102"/>
+      <c r="O1" s="102"/>
+      <c r="P1" s="102"/>
+    </row>
+    <row r="2" spans="1:18" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="103"/>
+      <c r="C2" s="103"/>
+      <c r="D2" s="103"/>
+      <c r="E2" s="103"/>
+      <c r="F2" s="103"/>
+      <c r="G2" s="103"/>
+      <c r="H2" s="103"/>
+      <c r="I2" s="103"/>
+      <c r="J2" s="103"/>
+      <c r="K2" s="103"/>
+      <c r="L2" s="103"/>
+      <c r="M2" s="103"/>
+      <c r="N2" s="103"/>
+      <c r="O2" s="103"/>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="94" t="s">
+      <c r="B3" s="104" t="s">
         <v>40</v>
       </c>
-      <c r="C3" s="94"/>
-      <c r="D3" s="94"/>
-      <c r="E3" s="94"/>
-      <c r="F3" s="94"/>
-      <c r="G3" s="94"/>
-      <c r="H3" s="94"/>
-      <c r="I3" s="94"/>
-      <c r="J3" s="94"/>
-      <c r="K3" s="94"/>
-      <c r="L3" s="94"/>
-      <c r="M3" s="94"/>
-      <c r="N3" s="94"/>
-      <c r="O3" s="94"/>
+      <c r="C3" s="104"/>
+      <c r="D3" s="104"/>
+      <c r="E3" s="104"/>
+      <c r="F3" s="104"/>
+      <c r="G3" s="104"/>
+      <c r="H3" s="104"/>
+      <c r="I3" s="104"/>
+      <c r="J3" s="104"/>
+      <c r="K3" s="104"/>
+      <c r="L3" s="104"/>
+      <c r="M3" s="104"/>
+      <c r="N3" s="104"/>
+      <c r="O3" s="104"/>
       <c r="P3" s="2"/>
       <c r="Q3" s="2"/>
       <c r="R3" s="2"/>
     </row>
-    <row r="4" spans="1:18" ht="5" customHeight="1">
+    <row r="4" spans="1:18" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
-      <c r="B4" s="95"/>
-      <c r="C4" s="95"/>
-      <c r="D4" s="95"/>
-      <c r="E4" s="95"/>
-      <c r="F4" s="95"/>
-      <c r="G4" s="95"/>
-      <c r="H4" s="95"/>
-      <c r="I4" s="95"/>
-      <c r="J4" s="95"/>
-      <c r="K4" s="95"/>
-      <c r="L4" s="95"/>
-      <c r="M4" s="95"/>
-      <c r="N4" s="95"/>
-      <c r="O4" s="95"/>
+      <c r="B4" s="105"/>
+      <c r="C4" s="105"/>
+      <c r="D4" s="105"/>
+      <c r="E4" s="105"/>
+      <c r="F4" s="105"/>
+      <c r="G4" s="105"/>
+      <c r="H4" s="105"/>
+      <c r="I4" s="105"/>
+      <c r="J4" s="105"/>
+      <c r="K4" s="105"/>
+      <c r="L4" s="105"/>
+      <c r="M4" s="105"/>
+      <c r="N4" s="105"/>
+      <c r="O4" s="105"/>
       <c r="P4" s="2"/>
       <c r="Q4" s="2"/>
       <c r="R4" s="2"/>
     </row>
-    <row r="5" spans="1:18">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
@@ -1137,7 +1183,7 @@
       <c r="Q5" s="2"/>
       <c r="R5" s="2"/>
     </row>
-    <row r="6" spans="1:18">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>3</v>
       </c>
@@ -1159,7 +1205,7 @@
       <c r="Q6" s="2"/>
       <c r="R6" s="2"/>
     </row>
-    <row r="7" spans="1:18" s="9" customFormat="1">
+    <row r="7" spans="1:18" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>41</v>
       </c>
@@ -1181,7 +1227,7 @@
       <c r="Q7" s="8"/>
       <c r="R7" s="8"/>
     </row>
-    <row r="8" spans="1:18" s="9" customFormat="1">
+    <row r="8" spans="1:18" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>42</v>
       </c>
@@ -1203,7 +1249,7 @@
       <c r="Q8" s="8"/>
       <c r="R8" s="8"/>
     </row>
-    <row r="9" spans="1:18" s="9" customFormat="1">
+    <row r="9" spans="1:18" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>44</v>
       </c>
@@ -1225,17 +1271,17 @@
       <c r="Q9" s="8"/>
       <c r="R9" s="8"/>
     </row>
-    <row r="10" spans="1:18">
-      <c r="A10" s="96" t="s">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A10" s="92" t="s">
         <v>4</v>
       </c>
-      <c r="B10" s="96"/>
-      <c r="C10" s="96"/>
-      <c r="D10" s="96"/>
-      <c r="E10" s="96"/>
-      <c r="F10" s="96"/>
-      <c r="G10" s="96"/>
-      <c r="H10" s="96"/>
+      <c r="B10" s="92"/>
+      <c r="C10" s="92"/>
+      <c r="D10" s="92"/>
+      <c r="E10" s="92"/>
+      <c r="F10" s="92"/>
+      <c r="G10" s="92"/>
+      <c r="H10" s="92"/>
       <c r="I10" s="4"/>
       <c r="J10" s="5"/>
       <c r="K10" s="5"/>
@@ -1247,17 +1293,17 @@
       <c r="Q10" s="2"/>
       <c r="R10" s="2"/>
     </row>
-    <row r="11" spans="1:18">
-      <c r="A11" s="96" t="s">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A11" s="92" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="96"/>
-      <c r="C11" s="96"/>
-      <c r="D11" s="96"/>
-      <c r="E11" s="96"/>
-      <c r="F11" s="96"/>
-      <c r="G11" s="96"/>
-      <c r="H11" s="96"/>
+      <c r="B11" s="92"/>
+      <c r="C11" s="92"/>
+      <c r="D11" s="92"/>
+      <c r="E11" s="92"/>
+      <c r="F11" s="92"/>
+      <c r="G11" s="92"/>
+      <c r="H11" s="92"/>
       <c r="I11" s="4"/>
       <c r="J11" s="5"/>
       <c r="K11" s="5"/>
@@ -1269,17 +1315,17 @@
       <c r="Q11" s="2"/>
       <c r="R11" s="2"/>
     </row>
-    <row r="12" spans="1:18">
-      <c r="A12" s="96" t="s">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A12" s="92" t="s">
         <v>43</v>
       </c>
-      <c r="B12" s="96"/>
-      <c r="C12" s="96"/>
-      <c r="D12" s="96"/>
-      <c r="E12" s="96"/>
-      <c r="F12" s="96"/>
-      <c r="G12" s="96"/>
-      <c r="H12" s="96"/>
+      <c r="B12" s="92"/>
+      <c r="C12" s="92"/>
+      <c r="D12" s="92"/>
+      <c r="E12" s="92"/>
+      <c r="F12" s="92"/>
+      <c r="G12" s="92"/>
+      <c r="H12" s="92"/>
       <c r="I12" s="4"/>
       <c r="J12" s="5"/>
       <c r="K12" s="5"/>
@@ -1291,27 +1337,27 @@
       <c r="Q12" s="2"/>
       <c r="R12" s="2"/>
     </row>
-    <row r="13" spans="1:18" ht="10" customHeight="1">
+    <row r="13" spans="1:18" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="10"/>
-      <c r="B13" s="95"/>
-      <c r="C13" s="95"/>
-      <c r="D13" s="95"/>
-      <c r="E13" s="95"/>
-      <c r="F13" s="95"/>
-      <c r="G13" s="95"/>
-      <c r="H13" s="95"/>
-      <c r="I13" s="95"/>
-      <c r="J13" s="95"/>
-      <c r="K13" s="95"/>
-      <c r="L13" s="95"/>
-      <c r="M13" s="95"/>
-      <c r="N13" s="95"/>
-      <c r="O13" s="95"/>
+      <c r="B13" s="105"/>
+      <c r="C13" s="105"/>
+      <c r="D13" s="105"/>
+      <c r="E13" s="105"/>
+      <c r="F13" s="105"/>
+      <c r="G13" s="105"/>
+      <c r="H13" s="105"/>
+      <c r="I13" s="105"/>
+      <c r="J13" s="105"/>
+      <c r="K13" s="105"/>
+      <c r="L13" s="105"/>
+      <c r="M13" s="105"/>
+      <c r="N13" s="105"/>
+      <c r="O13" s="105"/>
       <c r="P13" s="2"/>
       <c r="Q13" s="2"/>
       <c r="R13" s="2"/>
     </row>
-    <row r="14" spans="1:18">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="11"/>
       <c r="D14" s="12"/>
       <c r="E14" s="12"/>
@@ -1323,11 +1369,11 @@
       <c r="L14" s="12"/>
       <c r="N14" s="12"/>
     </row>
-    <row r="15" spans="1:18" s="16" customFormat="1">
+    <row r="15" spans="1:18" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="B15" s="104">
+      <c r="B15" s="100">
         <v>2012</v>
       </c>
       <c r="C15" s="14" t="s">
@@ -1371,7 +1417,7 @@
       </c>
       <c r="P15"/>
     </row>
-    <row r="16" spans="1:18" s="21" customFormat="1" ht="30">
+    <row r="16" spans="1:18" s="21" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A16" s="17" t="s">
         <v>9</v>
       </c>
@@ -1420,8 +1466,11 @@
       <c r="P16" s="20" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="17" spans="1:26" s="30" customFormat="1" ht="15" customHeight="1">
+      <c r="Q16" s="21" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="17" spans="1:26" s="30" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="22" t="s">
         <v>25</v>
       </c>
@@ -1455,8 +1504,6 @@
         <f>SUM(C17:O17)</f>
         <v>9479.74</v>
       </c>
-      <c r="Q17" s="28"/>
-      <c r="R17" s="29"/>
       <c r="S17" s="29"/>
       <c r="T17" s="29"/>
       <c r="U17" s="29"/>
@@ -1466,7 +1513,7 @@
       <c r="Y17" s="29"/>
       <c r="Z17" s="29"/>
     </row>
-    <row r="18" spans="1:26" s="30" customFormat="1">
+    <row r="18" spans="1:26" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="31" t="str">
         <f>A17</f>
         <v>Japan RESELLER</v>
@@ -1501,14 +1548,26 @@
         <f t="shared" ref="P18:P22" si="0">SUM(C18:O18)</f>
         <v>6548.92</v>
       </c>
-      <c r="Q18" s="28"/>
-      <c r="R18" s="29"/>
-      <c r="S18" s="29"/>
-      <c r="T18" s="29"/>
-      <c r="U18" s="29"/>
-      <c r="V18" s="29"/>
-    </row>
-    <row r="19" spans="1:26" s="30" customFormat="1">
+      <c r="Q18" s="106">
+        <v>1</v>
+      </c>
+      <c r="R18" s="106">
+        <v>2</v>
+      </c>
+      <c r="S18" s="106">
+        <v>3</v>
+      </c>
+      <c r="T18" s="106">
+        <v>4</v>
+      </c>
+      <c r="U18" s="106">
+        <v>5</v>
+      </c>
+      <c r="V18" s="29" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="19" spans="1:26" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="31" t="str">
         <f>A18</f>
         <v>Japan RESELLER</v>
@@ -1543,14 +1602,32 @@
         <f t="shared" si="0"/>
         <v>2660.23</v>
       </c>
-      <c r="Q19" s="28"/>
-      <c r="R19" s="29"/>
-      <c r="S19" s="29"/>
-      <c r="T19" s="29"/>
-      <c r="U19" s="29"/>
-      <c r="V19" s="29"/>
-    </row>
-    <row r="20" spans="1:26" s="30" customFormat="1">
+      <c r="Q19" s="28">
+        <f>C19/C$17</f>
+        <v>0.28362573099415206</v>
+      </c>
+      <c r="R19" s="28">
+        <f t="shared" ref="R19:U21" si="1">D19/D$17</f>
+        <v>0.27972372964972864</v>
+      </c>
+      <c r="S19" s="28">
+        <f t="shared" si="1"/>
+        <v>0.27960526315789475</v>
+      </c>
+      <c r="T19" s="28">
+        <f t="shared" si="1"/>
+        <v>0.27953714981729599</v>
+      </c>
+      <c r="U19" s="28">
+        <f t="shared" si="1"/>
+        <v>0.27953714981729594</v>
+      </c>
+      <c r="V19" s="28">
+        <f>AVERAGE(Q19:U19)</f>
+        <v>0.28040580468727344</v>
+      </c>
+    </row>
+    <row r="20" spans="1:26" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="31" t="str">
         <f>A19</f>
         <v>Japan RESELLER</v>
@@ -1585,14 +1662,32 @@
         <f t="shared" si="0"/>
         <v>4926.68</v>
       </c>
-      <c r="Q20" s="28"/>
-      <c r="R20" s="29"/>
-      <c r="S20" s="29"/>
-      <c r="T20" s="29"/>
-      <c r="U20" s="29"/>
-      <c r="V20" s="29"/>
-    </row>
-    <row r="21" spans="1:26" s="30" customFormat="1">
+      <c r="Q20" s="28">
+        <f t="shared" ref="Q20:Q21" si="2">C20/C$17</f>
+        <v>0.53675856307435255</v>
+      </c>
+      <c r="R20" s="28">
+        <f t="shared" si="1"/>
+        <v>0.51406018746916626</v>
+      </c>
+      <c r="S20" s="28">
+        <f t="shared" si="1"/>
+        <v>0.51370614035087714</v>
+      </c>
+      <c r="T20" s="28">
+        <f t="shared" si="1"/>
+        <v>0.51400730816077955</v>
+      </c>
+      <c r="U20" s="28">
+        <f t="shared" si="1"/>
+        <v>0.51400730816077955</v>
+      </c>
+      <c r="V20" s="28">
+        <f t="shared" ref="V20:V30" si="3">AVERAGE(Q20:U20)</f>
+        <v>0.51850790144319103</v>
+      </c>
+    </row>
+    <row r="21" spans="1:26" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="31" t="str">
         <f>A20</f>
         <v>Japan RESELLER</v>
@@ -1627,14 +1722,32 @@
         <f t="shared" si="0"/>
         <v>7541.09</v>
       </c>
-      <c r="Q21" s="28"/>
-      <c r="R21" s="29"/>
-      <c r="S21" s="29"/>
-      <c r="T21" s="29"/>
-      <c r="U21" s="29"/>
-      <c r="V21" s="29"/>
-    </row>
-    <row r="22" spans="1:26" s="42" customFormat="1">
+      <c r="Q21" s="28">
+        <f t="shared" si="2"/>
+        <v>0.81161236424394323</v>
+      </c>
+      <c r="R21" s="28">
+        <f t="shared" si="1"/>
+        <v>0.79033053774050321</v>
+      </c>
+      <c r="S21" s="28">
+        <f t="shared" si="1"/>
+        <v>0.79002192982456143</v>
+      </c>
+      <c r="T21" s="28">
+        <f t="shared" si="1"/>
+        <v>0.78989037758830694</v>
+      </c>
+      <c r="U21" s="28">
+        <f t="shared" si="1"/>
+        <v>0.78989037758830694</v>
+      </c>
+      <c r="V21" s="28">
+        <f t="shared" si="3"/>
+        <v>0.79434911739712444</v>
+      </c>
+    </row>
+    <row r="22" spans="1:26" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="37" t="str">
         <f>A21</f>
         <v>Japan RESELLER</v>
@@ -1643,83 +1756,85 @@
         <v>31</v>
       </c>
       <c r="C22" s="39">
-        <f t="shared" ref="C22:O22" si="1">SUM(C17:C21)</f>
+        <f t="shared" ref="C22:O22" si="4">SUM(C17:C21)</f>
         <v>7946</v>
       </c>
       <c r="D22" s="39">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>6641</v>
       </c>
       <c r="E22" s="39">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>5975</v>
       </c>
       <c r="F22" s="39">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>5378</v>
       </c>
       <c r="G22" s="39">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>5216.66</v>
       </c>
       <c r="H22" s="39">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="I22" s="39">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="J22" s="39">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K22" s="39">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="L22" s="39">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="M22" s="39">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="N22" s="39">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="O22" s="40">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="P22" s="41">
         <f t="shared" si="0"/>
         <v>31156.66</v>
       </c>
-    </row>
-    <row r="23" spans="1:26" s="100" customFormat="1">
-      <c r="A23" s="97"/>
-      <c r="B23" s="98"/>
-      <c r="C23" s="101"/>
-      <c r="D23" s="101"/>
-      <c r="E23" s="101"/>
-      <c r="F23" s="101"/>
-      <c r="G23" s="101"/>
-      <c r="H23" s="101"/>
-      <c r="I23" s="101"/>
-      <c r="J23" s="101"/>
-      <c r="K23" s="101"/>
-      <c r="L23" s="101"/>
-      <c r="M23" s="101"/>
-      <c r="N23" s="101"/>
-      <c r="O23" s="102"/>
-      <c r="P23" s="99"/>
-    </row>
-    <row r="24" spans="1:26" s="100" customFormat="1">
-      <c r="A24" s="97"/>
-      <c r="B24" s="98"/>
+      <c r="V22" s="28"/>
+    </row>
+    <row r="23" spans="1:26" s="96" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="93"/>
+      <c r="B23" s="94"/>
+      <c r="C23" s="97"/>
+      <c r="D23" s="97"/>
+      <c r="E23" s="97"/>
+      <c r="F23" s="97"/>
+      <c r="G23" s="97"/>
+      <c r="H23" s="97"/>
+      <c r="I23" s="97"/>
+      <c r="J23" s="97"/>
+      <c r="K23" s="97"/>
+      <c r="L23" s="97"/>
+      <c r="M23" s="97"/>
+      <c r="N23" s="97"/>
+      <c r="O23" s="98"/>
+      <c r="P23" s="95"/>
+      <c r="V23" s="28"/>
+    </row>
+    <row r="24" spans="1:26" s="96" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="93"/>
+      <c r="B24" s="94"/>
       <c r="C24" s="3" t="s">
         <v>7</v>
       </c>
@@ -1756,14 +1871,15 @@
       <c r="N24" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="O24" s="103" t="s">
-        <v>7</v>
-      </c>
-      <c r="P24" s="99"/>
-    </row>
-    <row r="25" spans="1:26" ht="30">
+      <c r="O24" s="99" t="s">
+        <v>7</v>
+      </c>
+      <c r="P24" s="95"/>
+      <c r="V24" s="28"/>
+    </row>
+    <row r="25" spans="1:26" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A25" s="43"/>
-      <c r="B25" s="105">
+      <c r="B25" s="101">
         <v>2011</v>
       </c>
       <c r="C25" s="18" t="s">
@@ -1806,8 +1922,12 @@
         <v>23</v>
       </c>
       <c r="P25" s="45"/>
-    </row>
-    <row r="26" spans="1:26" s="51" customFormat="1">
+      <c r="Q25" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="V25" s="28"/>
+    </row>
+    <row r="26" spans="1:26" s="51" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="46" t="s">
         <v>32</v>
       </c>
@@ -1858,7 +1978,7 @@
         <v>101087.70107538856</v>
       </c>
     </row>
-    <row r="27" spans="1:26" s="57" customFormat="1">
+    <row r="27" spans="1:26" s="57" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="52" t="s">
         <v>33</v>
       </c>
@@ -1877,8 +1997,26 @@
       <c r="N27" s="54"/>
       <c r="O27" s="55"/>
       <c r="P27" s="56"/>
-    </row>
-    <row r="28" spans="1:26" s="57" customFormat="1">
+      <c r="Q27" s="107">
+        <v>1</v>
+      </c>
+      <c r="R27" s="108">
+        <v>2</v>
+      </c>
+      <c r="S27" s="108">
+        <v>3</v>
+      </c>
+      <c r="T27" s="108">
+        <v>4</v>
+      </c>
+      <c r="U27" s="108">
+        <v>5</v>
+      </c>
+      <c r="V27" s="109" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="28" spans="1:26" s="57" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="52"/>
       <c r="B28" s="53"/>
       <c r="C28" s="54"/>
@@ -1895,8 +2033,32 @@
       <c r="N28" s="58"/>
       <c r="O28" s="59"/>
       <c r="P28" s="60"/>
-    </row>
-    <row r="29" spans="1:26" s="57" customFormat="1">
+      <c r="Q28" s="28">
+        <f>C19/C$18</f>
+        <v>0.4127659574468085</v>
+      </c>
+      <c r="R28" s="28">
+        <f>D19/D$18</f>
+        <v>0.40413399857448323</v>
+      </c>
+      <c r="S28" s="28">
+        <f>E19/E$18</f>
+        <v>0.40380047505938244</v>
+      </c>
+      <c r="T28" s="28">
+        <f>F19/F$18</f>
+        <v>0.40404929577464788</v>
+      </c>
+      <c r="U28" s="28">
+        <f>G19/G$18</f>
+        <v>0.40404929577464782</v>
+      </c>
+      <c r="V28" s="28">
+        <f>AVERAGE(Q28:U28)</f>
+        <v>0.40575980452599403</v>
+      </c>
+    </row>
+    <row r="29" spans="1:26" s="57" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="61"/>
       <c r="B29" s="53"/>
       <c r="C29" s="53"/>
@@ -1913,8 +2075,32 @@
       <c r="N29" s="53"/>
       <c r="O29" s="62"/>
       <c r="P29" s="63"/>
-    </row>
-    <row r="30" spans="1:26" s="57" customFormat="1">
+      <c r="Q29" s="28">
+        <f>C20/C$18</f>
+        <v>0.78115501519756836</v>
+      </c>
+      <c r="R29" s="28">
+        <f>D20/D$18</f>
+        <v>0.74269422665716323</v>
+      </c>
+      <c r="S29" s="28">
+        <f>E20/E$18</f>
+        <v>0.74188440221694374</v>
+      </c>
+      <c r="T29" s="28">
+        <f>F20/F$18</f>
+        <v>0.74295774647887325</v>
+      </c>
+      <c r="U29" s="28">
+        <f>G20/G$18</f>
+        <v>0.74295774647887314</v>
+      </c>
+      <c r="V29" s="28">
+        <f>AVERAGE(Q29:U29)</f>
+        <v>0.75032982740588428</v>
+      </c>
+    </row>
+    <row r="30" spans="1:26" s="57" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="61"/>
       <c r="B30" s="53"/>
       <c r="C30" s="53"/>
@@ -1931,9 +2117,32 @@
       <c r="N30" s="53"/>
       <c r="O30" s="62"/>
       <c r="P30" s="63"/>
-      <c r="S30" s="64"/>
-    </row>
-    <row r="31" spans="1:26" s="57" customFormat="1">
+      <c r="Q30" s="28">
+        <f>C21/C$18</f>
+        <v>1.1811550151975685</v>
+      </c>
+      <c r="R30" s="28">
+        <f>D21/D$18</f>
+        <v>1.1418389166072702</v>
+      </c>
+      <c r="S30" s="28">
+        <f>E21/E$18</f>
+        <v>1.1409342834520981</v>
+      </c>
+      <c r="T30" s="28">
+        <f>F21/F$18</f>
+        <v>1.141725352112676</v>
+      </c>
+      <c r="U30" s="28">
+        <f>G21/G$18</f>
+        <v>1.141725352112676</v>
+      </c>
+      <c r="V30" s="28">
+        <f>AVERAGE(Q30:U30)</f>
+        <v>1.1494757838964578</v>
+      </c>
+    </row>
+    <row r="31" spans="1:26" s="57" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="65"/>
       <c r="B31" s="66"/>
       <c r="C31" s="66"/>
@@ -1951,7 +2160,7 @@
       <c r="O31" s="67"/>
       <c r="P31" s="68"/>
     </row>
-    <row r="32" spans="1:26">
+    <row r="32" spans="1:26" x14ac:dyDescent="0.25">
       <c r="C32" s="12"/>
       <c r="H32" s="12"/>
       <c r="I32" s="12"/>
@@ -1962,11 +2171,11 @@
       <c r="N32" s="12"/>
       <c r="O32" s="12"/>
     </row>
-    <row r="33" spans="1:22" s="16" customFormat="1">
+    <row r="33" spans="1:28" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="B33" s="104">
+      <c r="B33" s="100">
         <v>2012</v>
       </c>
       <c r="C33" s="14" t="s">
@@ -2010,7 +2219,7 @@
       </c>
       <c r="P33"/>
     </row>
-    <row r="34" spans="1:22" s="21" customFormat="1" ht="30">
+    <row r="34" spans="1:28" s="21" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A34" s="17" t="s">
         <v>9</v>
       </c>
@@ -2059,8 +2268,11 @@
       <c r="P34" s="20" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="35" spans="1:22">
+      <c r="Q34" s="21" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="35" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A35" s="69" t="s">
         <v>34</v>
       </c>
@@ -2094,14 +2306,13 @@
         <f>SUM(C35:O35)</f>
         <v>8337.4313299999994</v>
       </c>
-      <c r="Q35" s="64"/>
       <c r="R35" s="71"/>
       <c r="S35" s="71"/>
       <c r="T35" s="71"/>
       <c r="U35" s="71"/>
       <c r="V35" s="71"/>
     </row>
-    <row r="36" spans="1:22">
+    <row r="36" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A36" s="31" t="str">
         <f>A35</f>
         <v>South Asia RESELLER</v>
@@ -2133,17 +2344,16 @@
       <c r="N36" s="34"/>
       <c r="O36" s="35"/>
       <c r="P36" s="36">
-        <f t="shared" ref="P36:P39" si="2">SUM(C36:O36)</f>
+        <f t="shared" ref="P36:P39" si="5">SUM(C36:O36)</f>
         <v>4856.0241800000003</v>
       </c>
-      <c r="Q36" s="64"/>
       <c r="R36" s="71"/>
       <c r="S36" s="71"/>
       <c r="T36" s="71"/>
       <c r="U36" s="71"/>
       <c r="V36" s="71"/>
     </row>
-    <row r="37" spans="1:22">
+    <row r="37" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A37" s="31" t="str">
         <f>A36</f>
         <v>South Asia RESELLER</v>
@@ -2151,11 +2361,21 @@
       <c r="B37" s="32" t="s">
         <v>28</v>
       </c>
-      <c r="C37" s="72"/>
-      <c r="D37" s="72"/>
-      <c r="E37" s="72"/>
-      <c r="F37" s="72"/>
-      <c r="G37" s="72"/>
+      <c r="C37" s="72">
+        <v>644.46577377353583</v>
+      </c>
+      <c r="D37" s="72">
+        <v>547.74726335463015</v>
+      </c>
+      <c r="E37" s="72">
+        <v>492.9951117224067</v>
+      </c>
+      <c r="F37" s="72">
+        <v>443.60425222792458</v>
+      </c>
+      <c r="G37" s="72">
+        <v>430.29612466108676</v>
+      </c>
       <c r="H37" s="34"/>
       <c r="I37" s="34"/>
       <c r="J37" s="34"/>
@@ -2165,16 +2385,35 @@
       <c r="N37" s="34"/>
       <c r="O37" s="35"/>
       <c r="P37" s="36">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="R37" s="29"/>
-      <c r="S37" s="29"/>
-      <c r="T37" s="29"/>
-      <c r="U37" s="29"/>
-      <c r="V37" s="29"/>
-    </row>
-    <row r="38" spans="1:22">
+        <f t="shared" si="5"/>
+        <v>2559.1085257395839</v>
+      </c>
+      <c r="Q37" s="64">
+        <f>AVERAGE(V19,V55)</f>
+        <v>0.29315152308214953</v>
+      </c>
+      <c r="R37" s="29">
+        <f>$Q37*C$35</f>
+        <v>617.23727433449676</v>
+      </c>
+      <c r="S37" s="29">
+        <f>$Q37*D$35</f>
+        <v>522.61485174437121</v>
+      </c>
+      <c r="T37" s="29">
+        <f>$Q37*E$35</f>
+        <v>470.27601854056894</v>
+      </c>
+      <c r="U37" s="29">
+        <f>$Q37*F$35</f>
+        <v>423.35154739233241</v>
+      </c>
+      <c r="V37" s="29">
+        <f t="shared" ref="S37:V39" si="6">$Q37*G$35</f>
+        <v>410.65100097056239</v>
+      </c>
+    </row>
+    <row r="38" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A38" s="31" t="str">
         <f>A37</f>
         <v>South Asia RESELLER</v>
@@ -2182,11 +2421,21 @@
       <c r="B38" s="32" t="s">
         <v>29</v>
       </c>
-      <c r="C38" s="72"/>
-      <c r="D38" s="72"/>
-      <c r="E38" s="72"/>
-      <c r="F38" s="72"/>
-      <c r="G38" s="72"/>
+      <c r="C38" s="72">
+        <v>846.73215015119524</v>
+      </c>
+      <c r="D38" s="72">
+        <v>719.55740031770188</v>
+      </c>
+      <c r="E38" s="72">
+        <v>647.62629686242371</v>
+      </c>
+      <c r="F38" s="72">
+        <v>582.75332407497592</v>
+      </c>
+      <c r="G38" s="72">
+        <v>565.27072435272657</v>
+      </c>
       <c r="H38" s="34"/>
       <c r="I38" s="34"/>
       <c r="J38" s="34"/>
@@ -2196,16 +2445,35 @@
       <c r="N38" s="34"/>
       <c r="O38" s="35"/>
       <c r="P38" s="36">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="R38" s="29"/>
-      <c r="S38" s="29"/>
-      <c r="T38" s="29"/>
-      <c r="U38" s="29"/>
-      <c r="V38" s="29"/>
-    </row>
-    <row r="39" spans="1:22">
+        <f t="shared" si="5"/>
+        <v>3361.9398957590233</v>
+      </c>
+      <c r="Q38" s="64">
+        <f>AVERAGE(V20,V56)</f>
+        <v>0.40066519656973848</v>
+      </c>
+      <c r="R38" s="29">
+        <f>$Q38*C$35</f>
+        <v>843.60978667710549</v>
+      </c>
+      <c r="S38" s="29">
+        <f t="shared" si="6"/>
+        <v>714.28447685651315</v>
+      </c>
+      <c r="T38" s="29">
+        <f t="shared" si="6"/>
+        <v>642.75031365874702</v>
+      </c>
+      <c r="U38" s="29">
+        <f>$Q38*F$35</f>
+        <v>578.61623630902557</v>
+      </c>
+      <c r="V38" s="29">
+        <f t="shared" si="6"/>
+        <v>561.25774921975483</v>
+      </c>
+    </row>
+    <row r="39" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A39" s="31" t="str">
         <f>A38</f>
         <v>South Asia RESELLER</v>
@@ -2213,11 +2481,21 @@
       <c r="B39" s="32" t="s">
         <v>30</v>
       </c>
-      <c r="C39" s="72"/>
-      <c r="D39" s="72"/>
-      <c r="E39" s="72"/>
-      <c r="F39" s="72"/>
-      <c r="G39" s="72"/>
+      <c r="C39" s="72">
+        <v>1737.6057990050517</v>
+      </c>
+      <c r="D39" s="72">
+        <v>1476.808010215886</v>
+      </c>
+      <c r="E39" s="72">
+        <v>1329.1867938293526</v>
+      </c>
+      <c r="F39" s="72">
+        <v>1196.0242891239759</v>
+      </c>
+      <c r="G39" s="72">
+        <v>1160.1435604502567</v>
+      </c>
       <c r="H39" s="34"/>
       <c r="I39" s="34"/>
       <c r="J39" s="34"/>
@@ -2227,16 +2505,35 @@
       <c r="N39" s="34"/>
       <c r="O39" s="35"/>
       <c r="P39" s="36">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="R39" s="29"/>
-      <c r="S39" s="29"/>
-      <c r="T39" s="29"/>
-      <c r="U39" s="29"/>
-      <c r="V39" s="29"/>
-    </row>
-    <row r="40" spans="1:22" s="42" customFormat="1">
+        <f t="shared" si="5"/>
+        <v>6899.768452624523</v>
+      </c>
+      <c r="Q39" s="64">
+        <f>AVERAGE(V21,V57)</f>
+        <v>0.79434911739712444</v>
+      </c>
+      <c r="R39" s="29">
+        <f>$Q39*C$35</f>
+        <v>1672.5203367093457</v>
+      </c>
+      <c r="S39" s="29">
+        <f>$Q39*D$35</f>
+        <v>1416.1231088178124</v>
+      </c>
+      <c r="T39" s="29">
+        <f t="shared" si="6"/>
+        <v>1274.3012089214062</v>
+      </c>
+      <c r="U39" s="29">
+        <f t="shared" si="6"/>
+        <v>1147.1505400487661</v>
+      </c>
+      <c r="V39" s="29">
+        <f>$Q39*G$35</f>
+        <v>1112.7360238473029</v>
+      </c>
+    </row>
+    <row r="40" spans="1:28" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="37" t="str">
         <f>A39</f>
         <v>South Asia RESELLER</v>
@@ -2245,63 +2542,63 @@
         <v>31</v>
       </c>
       <c r="C40" s="39">
-        <f t="shared" ref="C40:O40" si="3">SUM(C35:C39)</f>
-        <v>3325.2905000000001</v>
+        <f t="shared" ref="C40:O40" si="7">SUM(C35:C39)</f>
+        <v>6554.0942229297834</v>
       </c>
       <c r="D40" s="39">
-        <f t="shared" si="3"/>
-        <v>2823.0709999999999</v>
+        <f t="shared" si="7"/>
+        <v>5567.1836738882175</v>
       </c>
       <c r="E40" s="39">
-        <f t="shared" si="3"/>
-        <v>2540.7224999999999</v>
+        <f t="shared" si="7"/>
+        <v>5010.530702414183</v>
       </c>
       <c r="F40" s="39">
-        <f t="shared" si="3"/>
-        <v>2286.4830000000002</v>
+        <f t="shared" si="7"/>
+        <v>4508.8648654268763</v>
       </c>
       <c r="G40" s="39">
-        <f t="shared" si="3"/>
-        <v>2217.8885099999998</v>
+        <f t="shared" si="7"/>
+        <v>4373.5989194640697</v>
       </c>
       <c r="H40" s="39">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="I40" s="39">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="J40" s="39">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="K40" s="39">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="L40" s="39">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="M40" s="39">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="N40" s="39">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="O40" s="40">
-        <f t="shared" si="3"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="P40" s="41">
         <f>SUM(C40:O40)</f>
-        <v>13193.45551</v>
-      </c>
-    </row>
-    <row r="41" spans="1:22">
+        <v>26014.272384123127</v>
+      </c>
+    </row>
+    <row r="41" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A41" s="43"/>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
@@ -2319,9 +2616,9 @@
       <c r="O41" s="44"/>
       <c r="P41" s="45"/>
     </row>
-    <row r="42" spans="1:22" s="100" customFormat="1">
-      <c r="A42" s="97"/>
-      <c r="B42" s="98"/>
+    <row r="42" spans="1:28" s="96" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="93"/>
+      <c r="B42" s="94"/>
       <c r="C42" s="3" t="s">
         <v>7</v>
       </c>
@@ -2358,14 +2655,14 @@
       <c r="N42" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="O42" s="103" t="s">
-        <v>7</v>
-      </c>
-      <c r="P42" s="99"/>
-    </row>
-    <row r="43" spans="1:22" ht="30">
+      <c r="O42" s="99" t="s">
+        <v>7</v>
+      </c>
+      <c r="P42" s="95"/>
+    </row>
+    <row r="43" spans="1:28" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A43" s="43"/>
-      <c r="B43" s="105">
+      <c r="B43" s="101">
         <v>2011</v>
       </c>
       <c r="C43" s="18" t="s">
@@ -2408,8 +2705,14 @@
         <v>23</v>
       </c>
       <c r="P43" s="45"/>
-    </row>
-    <row r="44" spans="1:22" s="51" customFormat="1">
+      <c r="Q43" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="X43" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="44" spans="1:28" s="51" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="46" t="s">
         <v>32</v>
       </c>
@@ -2460,7 +2763,7 @@
         <v>43392.412699490647</v>
       </c>
     </row>
-    <row r="45" spans="1:22">
+    <row r="45" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A45" s="73" t="s">
         <v>33</v>
       </c>
@@ -2479,8 +2782,23 @@
       <c r="N45" s="54"/>
       <c r="O45" s="55"/>
       <c r="P45" s="56"/>
-    </row>
-    <row r="46" spans="1:22" s="57" customFormat="1">
+      <c r="X45">
+        <v>1</v>
+      </c>
+      <c r="Y45">
+        <v>2</v>
+      </c>
+      <c r="Z45">
+        <v>3</v>
+      </c>
+      <c r="AA45">
+        <v>4</v>
+      </c>
+      <c r="AB45">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="46" spans="1:28" s="57" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="61"/>
       <c r="B46" s="53"/>
       <c r="C46" s="54"/>
@@ -2497,8 +2815,52 @@
       <c r="N46" s="58"/>
       <c r="O46" s="59"/>
       <c r="P46" s="60"/>
-    </row>
-    <row r="47" spans="1:22" s="57" customFormat="1">
+      <c r="Q46" s="64">
+        <f>AVERAGE(V28,V64)</f>
+        <v>0.55067402042813474</v>
+      </c>
+      <c r="R46" s="29">
+        <f>$Q46*C$36</f>
+        <v>671.69427321257479</v>
+      </c>
+      <c r="S46" s="29">
+        <f t="shared" ref="S46:V48" si="8">$Q46*D$36</f>
+        <v>572.87967496488898</v>
+      </c>
+      <c r="T46" s="29">
+        <f t="shared" si="8"/>
+        <v>515.71420490424441</v>
+      </c>
+      <c r="U46" s="29">
+        <f t="shared" si="8"/>
+        <v>463.85695706351669</v>
+      </c>
+      <c r="V46" s="29">
+        <f t="shared" si="8"/>
+        <v>449.94124835161119</v>
+      </c>
+      <c r="X46" s="57">
+        <f>AVERAGE(R37, R46)</f>
+        <v>644.46577377353583</v>
+      </c>
+      <c r="Y46" s="57">
+        <f t="shared" ref="Y46:AB48" si="9">AVERAGE(S37, S46)</f>
+        <v>547.74726335463015</v>
+      </c>
+      <c r="Z46" s="57">
+        <f t="shared" si="9"/>
+        <v>492.9951117224067</v>
+      </c>
+      <c r="AA46" s="57">
+        <f t="shared" si="9"/>
+        <v>443.60425222792458</v>
+      </c>
+      <c r="AB46" s="57">
+        <f t="shared" si="9"/>
+        <v>430.29612466108676</v>
+      </c>
+    </row>
+    <row r="47" spans="1:28" s="57" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="61"/>
       <c r="B47" s="53"/>
       <c r="C47" s="53"/>
@@ -2515,8 +2877,52 @@
       <c r="N47" s="53"/>
       <c r="O47" s="62"/>
       <c r="P47" s="63"/>
-    </row>
-    <row r="48" spans="1:22" s="57" customFormat="1">
+      <c r="Q47" s="64">
+        <f t="shared" ref="Q47:Q48" si="10">AVERAGE(V29,V65)</f>
+        <v>0.69673483973403538</v>
+      </c>
+      <c r="R47" s="29">
+        <f>$Q47*C$36</f>
+        <v>849.85451362528499</v>
+      </c>
+      <c r="S47" s="29">
+        <f t="shared" si="8"/>
+        <v>724.83032377889049</v>
+      </c>
+      <c r="T47" s="29">
+        <f t="shared" si="8"/>
+        <v>652.5022800661003</v>
+      </c>
+      <c r="U47" s="29">
+        <f t="shared" si="8"/>
+        <v>586.89041184092628</v>
+      </c>
+      <c r="V47" s="29">
+        <f t="shared" si="8"/>
+        <v>569.28369948569843</v>
+      </c>
+      <c r="X47" s="57">
+        <f t="shared" ref="X47:X48" si="11">AVERAGE(R38, R47)</f>
+        <v>846.73215015119524</v>
+      </c>
+      <c r="Y47" s="57">
+        <f t="shared" si="9"/>
+        <v>719.55740031770188</v>
+      </c>
+      <c r="Z47" s="57">
+        <f t="shared" si="9"/>
+        <v>647.62629686242371</v>
+      </c>
+      <c r="AA47" s="57">
+        <f t="shared" si="9"/>
+        <v>582.75332407497592</v>
+      </c>
+      <c r="AB47" s="57">
+        <f t="shared" si="9"/>
+        <v>565.27072435272657</v>
+      </c>
+    </row>
+    <row r="48" spans="1:28" s="57" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="61"/>
       <c r="B48" s="53"/>
       <c r="C48" s="53"/>
@@ -2533,8 +2939,52 @@
       <c r="N48" s="53"/>
       <c r="O48" s="62"/>
       <c r="P48" s="63"/>
-    </row>
-    <row r="49" spans="1:17" s="57" customFormat="1">
+      <c r="Q48" s="64">
+        <f t="shared" si="10"/>
+        <v>1.4778974364383031</v>
+      </c>
+      <c r="R48" s="29">
+        <f>$Q48*C$36</f>
+        <v>1802.6912613007578</v>
+      </c>
+      <c r="S48" s="29">
+        <f t="shared" si="8"/>
+        <v>1537.4929116139594</v>
+      </c>
+      <c r="T48" s="29">
+        <f t="shared" si="8"/>
+        <v>1384.0723787372992</v>
+      </c>
+      <c r="U48" s="29">
+        <f t="shared" si="8"/>
+        <v>1244.898038199186</v>
+      </c>
+      <c r="V48" s="29">
+        <f t="shared" si="8"/>
+        <v>1207.5510970532102</v>
+      </c>
+      <c r="X48" s="57">
+        <f t="shared" si="11"/>
+        <v>1737.6057990050517</v>
+      </c>
+      <c r="Y48" s="57">
+        <f t="shared" si="9"/>
+        <v>1476.808010215886</v>
+      </c>
+      <c r="Z48" s="57">
+        <f t="shared" si="9"/>
+        <v>1329.1867938293526</v>
+      </c>
+      <c r="AA48" s="57">
+        <f t="shared" si="9"/>
+        <v>1196.0242891239759</v>
+      </c>
+      <c r="AB48" s="57">
+        <f t="shared" si="9"/>
+        <v>1160.1435604502567</v>
+      </c>
+    </row>
+    <row r="49" spans="1:22" s="57" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="65"/>
       <c r="B49" s="66"/>
       <c r="C49" s="66"/>
@@ -2552,7 +3002,7 @@
       <c r="O49" s="67"/>
       <c r="P49" s="68"/>
     </row>
-    <row r="50" spans="1:17">
+    <row r="50" spans="1:22" x14ac:dyDescent="0.25">
       <c r="C50" s="12"/>
       <c r="H50" s="12"/>
       <c r="I50" s="12"/>
@@ -2563,11 +3013,11 @@
       <c r="N50" s="12"/>
       <c r="O50" s="12"/>
     </row>
-    <row r="51" spans="1:17" s="16" customFormat="1">
+    <row r="51" spans="1:22" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="B51" s="104">
+      <c r="B51" s="100">
         <v>2012</v>
       </c>
       <c r="C51" s="14" t="s">
@@ -2611,7 +3061,7 @@
       </c>
       <c r="P51"/>
     </row>
-    <row r="52" spans="1:17" s="21" customFormat="1" ht="30">
+    <row r="52" spans="1:22" s="21" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A52" s="17" t="s">
         <v>9</v>
       </c>
@@ -2660,8 +3110,11 @@
       <c r="P52" s="20" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="53" spans="1:17">
+      <c r="Q52" s="21" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="53" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A53" s="69" t="s">
         <v>35</v>
       </c>
@@ -2695,9 +3148,14 @@
         <f>SUM(C53:O53)</f>
         <v>7195.12266</v>
       </c>
-      <c r="Q53" s="64"/>
-    </row>
-    <row r="54" spans="1:17">
+      <c r="Q53" s="30"/>
+      <c r="R53" s="30"/>
+      <c r="S53" s="29"/>
+      <c r="T53" s="29"/>
+      <c r="U53" s="29"/>
+      <c r="V53" s="29"/>
+    </row>
+    <row r="54" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A54" s="31" t="str">
         <f>A53</f>
         <v>ANZ RESELLER</v>
@@ -2729,12 +3187,29 @@
       <c r="N54" s="34"/>
       <c r="O54" s="35"/>
       <c r="P54" s="36">
-        <f t="shared" ref="P54:P58" si="4">SUM(C54:O54)</f>
+        <f t="shared" ref="P54:P58" si="12">SUM(C54:O54)</f>
         <v>3163.1283599999988</v>
       </c>
-      <c r="Q54" s="64"/>
-    </row>
-    <row r="55" spans="1:17">
+      <c r="Q54" s="106">
+        <v>1</v>
+      </c>
+      <c r="R54" s="106">
+        <v>2</v>
+      </c>
+      <c r="S54" s="106">
+        <v>3</v>
+      </c>
+      <c r="T54" s="106">
+        <v>4</v>
+      </c>
+      <c r="U54" s="106">
+        <v>5</v>
+      </c>
+      <c r="V54" s="29" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="55" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A55" s="31" t="str">
         <f>A54</f>
         <v>ANZ RESELLER</v>
@@ -2766,12 +3241,35 @@
       <c r="N55" s="34"/>
       <c r="O55" s="35"/>
       <c r="P55" s="36">
-        <f t="shared" si="4"/>
+        <f t="shared" si="12"/>
         <v>2202.6704399999999</v>
       </c>
-      <c r="Q55" s="64"/>
-    </row>
-    <row r="56" spans="1:17">
+      <c r="Q55" s="28">
+        <f>C55/C$53</f>
+        <v>0.30940988835725669</v>
+      </c>
+      <c r="R55" s="28">
+        <f t="shared" ref="R55:U57" si="13">D55/D$53</f>
+        <v>0.30515315961788586</v>
+      </c>
+      <c r="S55" s="28">
+        <f t="shared" si="13"/>
+        <v>0.30502392344497609</v>
+      </c>
+      <c r="T55" s="28">
+        <f t="shared" si="13"/>
+        <v>0.30494961798250464</v>
+      </c>
+      <c r="U55" s="28">
+        <f t="shared" si="13"/>
+        <v>0.30494961798250458</v>
+      </c>
+      <c r="V55" s="28">
+        <f>AVERAGE(Q55:U55)</f>
+        <v>0.30589724147702557</v>
+      </c>
+    </row>
+    <row r="56" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A56" s="31" t="str">
         <f>A55</f>
         <v>ANZ RESELLER</v>
@@ -2803,12 +3301,35 @@
       <c r="N56" s="34"/>
       <c r="O56" s="35"/>
       <c r="P56" s="36">
-        <f t="shared" si="4"/>
+        <f t="shared" si="12"/>
         <v>2039.6455199999996</v>
       </c>
-      <c r="Q56" s="64"/>
-    </row>
-    <row r="57" spans="1:17">
+      <c r="Q56" s="28">
+        <f t="shared" ref="Q56:Q57" si="14">C56/C$53</f>
+        <v>0.29277739804055586</v>
+      </c>
+      <c r="R56" s="28">
+        <f t="shared" si="13"/>
+        <v>0.28039646589227252</v>
+      </c>
+      <c r="S56" s="28">
+        <f t="shared" si="13"/>
+        <v>0.28020334928229662</v>
+      </c>
+      <c r="T56" s="28">
+        <f t="shared" si="13"/>
+        <v>0.2803676226331524</v>
+      </c>
+      <c r="U56" s="28">
+        <f t="shared" si="13"/>
+        <v>0.28036762263315235</v>
+      </c>
+      <c r="V56" s="28">
+        <f t="shared" ref="V56:V57" si="15">AVERAGE(Q56:U56)</f>
+        <v>0.28282249169628593</v>
+      </c>
+    </row>
+    <row r="57" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A57" s="31" t="str">
         <f>A56</f>
         <v>ANZ RESELLER</v>
@@ -2840,12 +3361,35 @@
       <c r="N57" s="34"/>
       <c r="O57" s="35"/>
       <c r="P57" s="36">
-        <f t="shared" si="4"/>
+        <f t="shared" si="12"/>
         <v>5723.6873099999993</v>
       </c>
-      <c r="Q57" s="64"/>
-    </row>
-    <row r="58" spans="1:17" s="42" customFormat="1">
+      <c r="Q57" s="28">
+        <f t="shared" si="14"/>
+        <v>0.81161236424394312</v>
+      </c>
+      <c r="R57" s="28">
+        <f>D57/D$53</f>
+        <v>0.79033053774050344</v>
+      </c>
+      <c r="S57" s="28">
+        <f t="shared" si="13"/>
+        <v>0.79002192982456143</v>
+      </c>
+      <c r="T57" s="28">
+        <f t="shared" si="13"/>
+        <v>0.78989037758830694</v>
+      </c>
+      <c r="U57" s="28">
+        <f t="shared" si="13"/>
+        <v>0.78989037758830682</v>
+      </c>
+      <c r="V57" s="28">
+        <f t="shared" si="15"/>
+        <v>0.79434911739712444</v>
+      </c>
+    </row>
+    <row r="58" spans="1:22" s="42" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="37" t="str">
         <f>A57</f>
         <v>ANZ RESELLER</v>
@@ -2854,63 +3398,63 @@
         <v>31</v>
       </c>
       <c r="C58" s="39">
-        <f t="shared" ref="C58:O58" si="5">SUM(C53:C57)</f>
+        <f t="shared" ref="C58:O58" si="16">SUM(C53:C57)</f>
         <v>5180.5199999999995</v>
       </c>
       <c r="D58" s="39">
-        <f t="shared" si="5"/>
+        <f t="shared" si="16"/>
         <v>4332.9239999999991</v>
       </c>
       <c r="E58" s="39">
-        <f t="shared" si="5"/>
+        <f t="shared" si="16"/>
         <v>3898.3619999999996</v>
       </c>
       <c r="F58" s="39">
-        <f t="shared" si="5"/>
+        <f t="shared" si="16"/>
         <v>3508.857</v>
       </c>
       <c r="G58" s="39">
-        <f t="shared" si="5"/>
+        <f t="shared" si="16"/>
         <v>3403.5912899999998</v>
       </c>
       <c r="H58" s="39">
-        <f t="shared" si="5"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="I58" s="39">
-        <f t="shared" si="5"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="J58" s="39">
-        <f t="shared" si="5"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="K58" s="39">
-        <f t="shared" si="5"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="L58" s="39">
-        <f t="shared" si="5"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="M58" s="39">
-        <f t="shared" si="5"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="N58" s="39">
-        <f t="shared" si="5"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="O58" s="40">
-        <f t="shared" si="5"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="P58" s="41">
-        <f t="shared" si="4"/>
+        <f t="shared" si="12"/>
         <v>20324.254290000001</v>
       </c>
     </row>
-    <row r="59" spans="1:17">
+    <row r="59" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A59" s="43"/>
       <c r="B59" s="2"/>
       <c r="C59" s="2"/>
@@ -2928,9 +3472,9 @@
       <c r="O59" s="44"/>
       <c r="P59" s="45"/>
     </row>
-    <row r="60" spans="1:17" s="100" customFormat="1">
-      <c r="A60" s="97"/>
-      <c r="B60" s="98"/>
+    <row r="60" spans="1:22" s="96" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="93"/>
+      <c r="B60" s="94"/>
       <c r="C60" s="3" t="s">
         <v>7</v>
       </c>
@@ -2967,14 +3511,14 @@
       <c r="N60" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="O60" s="103" t="s">
-        <v>7</v>
-      </c>
-      <c r="P60" s="99"/>
-    </row>
-    <row r="61" spans="1:17" ht="30">
+      <c r="O60" s="99" t="s">
+        <v>7</v>
+      </c>
+      <c r="P60" s="95"/>
+    </row>
+    <row r="61" spans="1:22" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A61" s="43"/>
-      <c r="B61" s="105">
+      <c r="B61" s="101">
         <v>2011</v>
       </c>
       <c r="C61" s="18" t="s">
@@ -3017,8 +3561,12 @@
         <v>23</v>
       </c>
       <c r="P61" s="45"/>
-    </row>
-    <row r="62" spans="1:17" s="51" customFormat="1">
+      <c r="Q61" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="V61" s="28"/>
+    </row>
+    <row r="62" spans="1:22" s="51" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A62" s="46" t="s">
         <v>32</v>
       </c>
@@ -3069,7 +3617,7 @@
         <v>66645.686690430244</v>
       </c>
     </row>
-    <row r="63" spans="1:17" s="57" customFormat="1">
+    <row r="63" spans="1:22" s="57" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="52" t="s">
         <v>33</v>
       </c>
@@ -3088,8 +3636,26 @@
       <c r="N63" s="54"/>
       <c r="O63" s="55"/>
       <c r="P63" s="56"/>
-    </row>
-    <row r="64" spans="1:17" s="57" customFormat="1">
+      <c r="Q63" s="107">
+        <v>1</v>
+      </c>
+      <c r="R63" s="108">
+        <v>2</v>
+      </c>
+      <c r="S63" s="108">
+        <v>3</v>
+      </c>
+      <c r="T63" s="108">
+        <v>4</v>
+      </c>
+      <c r="U63" s="108">
+        <v>5</v>
+      </c>
+      <c r="V63" s="109" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="64" spans="1:22" s="57" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="61"/>
       <c r="B64" s="53"/>
       <c r="C64" s="54"/>
@@ -3106,8 +3672,32 @@
       <c r="N64" s="58"/>
       <c r="O64" s="59"/>
       <c r="P64" s="60"/>
-    </row>
-    <row r="65" spans="1:16" s="57" customFormat="1">
+      <c r="Q64" s="28">
+        <f>C55/C$54</f>
+        <v>0.70759878419452893</v>
+      </c>
+      <c r="R64" s="28">
+        <f t="shared" ref="R64:U66" si="17">D55/D$54</f>
+        <v>0.69280114041340002</v>
+      </c>
+      <c r="S64" s="28">
+        <f t="shared" si="17"/>
+        <v>0.69222938581608429</v>
+      </c>
+      <c r="T64" s="28">
+        <f t="shared" si="17"/>
+        <v>0.69265593561368211</v>
+      </c>
+      <c r="U64" s="28">
+        <f t="shared" si="17"/>
+        <v>0.69265593561368188</v>
+      </c>
+      <c r="V64" s="28">
+        <f>AVERAGE(Q64:U64)</f>
+        <v>0.69558823633027544</v>
+      </c>
+    </row>
+    <row r="65" spans="1:22" s="57" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="61"/>
       <c r="B65" s="53"/>
       <c r="C65" s="53"/>
@@ -3124,8 +3714,32 @@
       <c r="N65" s="53"/>
       <c r="O65" s="62"/>
       <c r="P65" s="63"/>
-    </row>
-    <row r="66" spans="1:16" s="57" customFormat="1">
+      <c r="Q65" s="28">
+        <f t="shared" ref="Q65:Q66" si="18">C56/C$54</f>
+        <v>0.66956144159791586</v>
+      </c>
+      <c r="R65" s="28">
+        <f t="shared" si="17"/>
+        <v>0.63659505142042572</v>
+      </c>
+      <c r="S65" s="28">
+        <f t="shared" si="17"/>
+        <v>0.6359009161859519</v>
+      </c>
+      <c r="T65" s="28">
+        <f t="shared" si="17"/>
+        <v>0.63682092555331993</v>
+      </c>
+      <c r="U65" s="28">
+        <f t="shared" si="17"/>
+        <v>0.63682092555331971</v>
+      </c>
+      <c r="V65" s="28">
+        <f>AVERAGE(Q65:U65)</f>
+        <v>0.64313985206218649</v>
+      </c>
+    </row>
+    <row r="66" spans="1:22" s="57" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" s="61"/>
       <c r="B66" s="53"/>
       <c r="C66" s="53"/>
@@ -3142,8 +3756,32 @@
       <c r="N66" s="53"/>
       <c r="O66" s="62"/>
       <c r="P66" s="63"/>
-    </row>
-    <row r="67" spans="1:16" s="57" customFormat="1">
+      <c r="Q66" s="28">
+        <f t="shared" si="18"/>
+        <v>1.8561007381676078</v>
+      </c>
+      <c r="R66" s="28">
+        <f t="shared" si="17"/>
+        <v>1.794318297525711</v>
+      </c>
+      <c r="S66" s="28">
+        <f t="shared" si="17"/>
+        <v>1.7928967311390118</v>
+      </c>
+      <c r="T66" s="28">
+        <f t="shared" si="17"/>
+        <v>1.7941398390342056</v>
+      </c>
+      <c r="U66" s="28">
+        <f t="shared" si="17"/>
+        <v>1.7941398390342052</v>
+      </c>
+      <c r="V66" s="28">
+        <f>AVERAGE(Q66:U66)</f>
+        <v>1.8063190889801484</v>
+      </c>
+    </row>
+    <row r="67" spans="1:22" s="57" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A67" s="65"/>
       <c r="B67" s="66"/>
       <c r="C67" s="66"/>
@@ -3161,11 +3799,11 @@
       <c r="O67" s="67"/>
       <c r="P67" s="68"/>
     </row>
-    <row r="69" spans="1:16" s="16" customFormat="1">
+    <row r="69" spans="1:22" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A69" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="B69" s="104">
+      <c r="B69" s="100">
         <v>2012</v>
       </c>
       <c r="C69" s="14" t="s">
@@ -3209,7 +3847,7 @@
       </c>
       <c r="P69"/>
     </row>
-    <row r="70" spans="1:16" s="21" customFormat="1" ht="30">
+    <row r="70" spans="1:22" s="21" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A70" s="17" t="s">
         <v>9</v>
       </c>
@@ -3259,7 +3897,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="71" spans="1:16">
+    <row r="71" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A71" s="69" t="s">
         <v>36</v>
       </c>
@@ -3284,7 +3922,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:16">
+    <row r="72" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A72" s="31" t="str">
         <f>A71</f>
         <v>China RESELLER</v>
@@ -3306,11 +3944,11 @@
       <c r="N72" s="34"/>
       <c r="O72" s="35"/>
       <c r="P72" s="36">
-        <f t="shared" ref="P72:P76" si="6">SUM(C72:O72)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="73" spans="1:16">
+        <f t="shared" ref="P72:P76" si="19">SUM(C72:O72)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A73" s="31" t="str">
         <f>A72</f>
         <v>China RESELLER</v>
@@ -3332,11 +3970,11 @@
       <c r="N73" s="34"/>
       <c r="O73" s="35"/>
       <c r="P73" s="36">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="74" spans="1:16">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A74" s="31" t="str">
         <f>A73</f>
         <v>China RESELLER</v>
@@ -3358,11 +3996,11 @@
       <c r="N74" s="34"/>
       <c r="O74" s="35"/>
       <c r="P74" s="36">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="75" spans="1:16">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A75" s="31" t="str">
         <f>A74</f>
         <v>China RESELLER</v>
@@ -3384,11 +4022,11 @@
       <c r="N75" s="34"/>
       <c r="O75" s="35"/>
       <c r="P75" s="36">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="76" spans="1:16">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A76" s="37" t="str">
         <f>A75</f>
         <v>China RESELLER</v>
@@ -3397,63 +4035,63 @@
         <v>31</v>
       </c>
       <c r="C76" s="39">
-        <f t="shared" ref="C76:O76" si="7">SUM(C71:C75)</f>
+        <f t="shared" ref="C76:O76" si="20">SUM(C71:C75)</f>
         <v>0</v>
       </c>
       <c r="D76" s="39">
-        <f t="shared" si="7"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="E76" s="39">
-        <f t="shared" si="7"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="F76" s="39">
-        <f t="shared" si="7"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="G76" s="39">
-        <f t="shared" si="7"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="H76" s="39">
-        <f t="shared" si="7"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="I76" s="39">
-        <f t="shared" si="7"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="J76" s="39">
-        <f t="shared" si="7"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="K76" s="39">
-        <f t="shared" si="7"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="L76" s="39">
-        <f t="shared" si="7"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="M76" s="39">
-        <f t="shared" si="7"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="N76" s="39">
-        <f t="shared" si="7"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="O76" s="40">
-        <f t="shared" si="7"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="P76" s="41">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="77" spans="1:16">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A77" s="74"/>
       <c r="B77" s="1"/>
       <c r="C77" s="75"/>
@@ -3471,9 +4109,9 @@
       <c r="O77" s="76"/>
       <c r="P77" s="45"/>
     </row>
-    <row r="78" spans="1:16" s="100" customFormat="1">
-      <c r="A78" s="97"/>
-      <c r="B78" s="98"/>
+    <row r="78" spans="1:22" s="96" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A78" s="93"/>
+      <c r="B78" s="94"/>
       <c r="C78" s="3" t="s">
         <v>7</v>
       </c>
@@ -3510,14 +4148,14 @@
       <c r="N78" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="O78" s="103" t="s">
-        <v>7</v>
-      </c>
-      <c r="P78" s="99"/>
-    </row>
-    <row r="79" spans="1:16" ht="30">
+      <c r="O78" s="99" t="s">
+        <v>7</v>
+      </c>
+      <c r="P78" s="95"/>
+    </row>
+    <row r="79" spans="1:22" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A79" s="43"/>
-      <c r="B79" s="105">
+      <c r="B79" s="101">
         <v>2011</v>
       </c>
       <c r="C79" s="18" t="s">
@@ -3561,7 +4199,7 @@
       </c>
       <c r="P79" s="45"/>
     </row>
-    <row r="80" spans="1:16">
+    <row r="80" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A80" s="77" t="s">
         <v>32</v>
       </c>
@@ -3612,7 +4250,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:16">
+    <row r="81" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A81" s="52" t="s">
         <v>33</v>
       </c>
@@ -3632,7 +4270,7 @@
       <c r="O81" s="55"/>
       <c r="P81" s="56"/>
     </row>
-    <row r="82" spans="1:16">
+    <row r="82" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A82" s="61"/>
       <c r="B82" s="53"/>
       <c r="C82" s="54"/>
@@ -3650,7 +4288,7 @@
       <c r="O82" s="59"/>
       <c r="P82" s="60"/>
     </row>
-    <row r="83" spans="1:16">
+    <row r="83" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A83" s="61"/>
       <c r="B83" s="53"/>
       <c r="C83" s="53"/>
@@ -3668,7 +4306,7 @@
       <c r="O83" s="62"/>
       <c r="P83" s="63"/>
     </row>
-    <row r="84" spans="1:16">
+    <row r="84" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A84" s="61"/>
       <c r="B84" s="53"/>
       <c r="C84" s="53"/>
@@ -3686,7 +4324,7 @@
       <c r="O84" s="62"/>
       <c r="P84" s="63"/>
     </row>
-    <row r="85" spans="1:16">
+    <row r="85" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A85" s="65"/>
       <c r="B85" s="66"/>
       <c r="C85" s="66"/>
@@ -3704,7 +4342,7 @@
       <c r="O85" s="67"/>
       <c r="P85" s="68"/>
     </row>
-    <row r="87" spans="1:16">
+    <row r="87" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A87" s="79" t="s">
         <v>37</v>
       </c>
@@ -3712,55 +4350,55 @@
         <v>26</v>
       </c>
       <c r="C87" s="81">
-        <f>C17+C35+C53+C71</f>
+        <f t="shared" ref="C87:O87" si="21">C17+C35+C53+C71</f>
         <v>6316.5690000000004</v>
       </c>
       <c r="D87" s="81">
-        <f>D17+D35+D53+D71</f>
+        <f t="shared" si="21"/>
         <v>5348.2394999999997</v>
       </c>
       <c r="E87" s="81">
-        <f>E17+E35+E53+E71</f>
+        <f t="shared" si="21"/>
         <v>4812.6239999999998</v>
       </c>
       <c r="F87" s="81">
-        <f>F17+F35+F53+F71</f>
+        <f t="shared" si="21"/>
         <v>4332.4170000000004</v>
       </c>
       <c r="G87" s="81">
-        <f>G17+G35+G53+G71</f>
+        <f t="shared" si="21"/>
         <v>4202.4444899999999</v>
       </c>
       <c r="H87" s="81">
-        <f>H17+H35+H53+H71</f>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="I87" s="81">
-        <f>I17+I35+I53+I71</f>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="J87" s="81">
-        <f>J17+J35+J53+J71</f>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="K87" s="81">
-        <f>K17+K35+K53+K71</f>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="L87" s="81">
-        <f>L17+L35+L53+L71</f>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="M87" s="81">
-        <f>M17+M35+M53+M71</f>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="N87" s="81">
-        <f>N17+N35+N53+N71</f>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="O87" s="82">
-        <f>O17+O35+O53+O71</f>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="P87" s="27">
@@ -3768,7 +4406,7 @@
         <v>25012.293989999998</v>
       </c>
     </row>
-    <row r="88" spans="1:16">
+    <row r="88" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A88" s="83" t="s">
         <v>37</v>
       </c>
@@ -3776,63 +4414,63 @@
         <v>27</v>
       </c>
       <c r="C88" s="85">
-        <f>C18+C36+C54+C72</f>
+        <f t="shared" ref="C88:O88" si="22">C18+C36+C54+C72</f>
         <v>3659.3024999999998</v>
       </c>
       <c r="D88" s="85">
-        <f>D18+D36+D54+D72</f>
+        <f t="shared" si="22"/>
         <v>3120.9734999999996</v>
       </c>
       <c r="E88" s="85">
-        <f>E18+E36+E54+E72</f>
+        <f t="shared" si="22"/>
         <v>2809.5435000000002</v>
       </c>
       <c r="F88" s="85">
-        <f>F18+F36+F54+F72</f>
+        <f t="shared" si="22"/>
         <v>2527.0320000000002</v>
       </c>
       <c r="G88" s="85">
-        <f>G18+G36+G54+G72</f>
+        <f t="shared" si="22"/>
         <v>2451.2210399999999</v>
       </c>
       <c r="H88" s="85">
-        <f>H18+H36+H54+H72</f>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="I88" s="85">
-        <f>I18+I36+I54+I72</f>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="J88" s="85">
-        <f>J18+J36+J54+J72</f>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="K88" s="85">
-        <f>K18+K36+K54+K72</f>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="L88" s="85">
-        <f>L18+L36+L54+L72</f>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="M88" s="85">
-        <f>M18+M36+M54+M72</f>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="N88" s="85">
-        <f>N18+N36+N54+N72</f>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="O88" s="86">
-        <f>O18+O36+O54+O72</f>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="P88" s="36">
-        <f t="shared" ref="P88:P92" si="8">SUM(C88:O88)</f>
+        <f t="shared" ref="P88:P92" si="23">SUM(C88:O88)</f>
         <v>14568.072540000001</v>
       </c>
     </row>
-    <row r="89" spans="1:16">
+    <row r="89" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A89" s="83" t="s">
         <v>37</v>
       </c>
@@ -3840,63 +4478,63 @@
         <v>38</v>
       </c>
       <c r="C89" s="85">
-        <f>C19+C37+C55+C73</f>
-        <v>1241.212</v>
+        <f t="shared" ref="C89:O89" si="24">C19+C37+C55+C73</f>
+        <v>1885.6777737735356</v>
       </c>
       <c r="D89" s="85">
-        <f>D19+D37+D55+D73</f>
-        <v>1036.4759999999999</v>
+        <f t="shared" si="24"/>
+        <v>1584.22326335463</v>
       </c>
       <c r="E89" s="85">
-        <f>E19+E37+E55+E73</f>
-        <v>932.28</v>
+        <f t="shared" si="24"/>
+        <v>1425.2751117224066</v>
       </c>
       <c r="F89" s="85">
-        <f>F19+F37+F55+F73</f>
-        <v>839.05199999999991</v>
+        <f t="shared" si="24"/>
+        <v>1282.6562522279246</v>
       </c>
       <c r="G89" s="85">
-        <f>G19+G37+G55+G73</f>
-        <v>813.88043999999991</v>
+        <f t="shared" si="24"/>
+        <v>1244.1765646610866</v>
       </c>
       <c r="H89" s="85">
-        <f>H19+H37+H55+H73</f>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="I89" s="85">
-        <f>I19+I37+I55+I73</f>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="J89" s="85">
-        <f>J19+J37+J55+J73</f>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="K89" s="85">
-        <f>K19+K37+K55+K73</f>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="L89" s="85">
-        <f>L19+L37+L55+L73</f>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="M89" s="85">
-        <f>M19+M37+M55+M73</f>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="N89" s="85">
-        <f>N19+N37+N55+N73</f>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="O89" s="86">
-        <f>O19+O37+O55+O73</f>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="P89" s="36">
-        <f t="shared" si="8"/>
-        <v>4862.9004399999994</v>
-      </c>
-    </row>
-    <row r="90" spans="1:16">
+        <f t="shared" si="23"/>
+        <v>7422.0089657395838</v>
+      </c>
+    </row>
+    <row r="90" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A90" s="83" t="s">
         <v>37</v>
       </c>
@@ -3904,63 +4542,63 @@
         <v>29</v>
       </c>
       <c r="C90" s="85">
-        <f>C20+C38+C56+C74</f>
-        <v>1816.9899999999998</v>
+        <f t="shared" ref="C90:O90" si="25">C20+C38+C56+C74</f>
+        <v>2663.7221501511949</v>
       </c>
       <c r="D90" s="85">
-        <f>D20+D38+D56+D74</f>
-        <v>1473.3879999999999</v>
+        <f t="shared" si="25"/>
+        <v>2192.9454003177016</v>
       </c>
       <c r="E90" s="85">
-        <f>E20+E38+E56+E74</f>
-        <v>1324.9179999999999</v>
+        <f t="shared" si="25"/>
+        <v>1972.5442968624236</v>
       </c>
       <c r="F90" s="85">
-        <f>F20+F38+F56+F74</f>
-        <v>1193.4159999999999</v>
+        <f t="shared" si="25"/>
+        <v>1776.1693240749757</v>
       </c>
       <c r="G90" s="85">
-        <f>G20+G38+G56+G74</f>
-        <v>1157.6135199999999</v>
+        <f t="shared" si="25"/>
+        <v>1722.8842443527262</v>
       </c>
       <c r="H90" s="85">
-        <f>H20+H38+H56+H74</f>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="I90" s="85">
-        <f>I20+I38+I56+I74</f>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="J90" s="85">
-        <f>J20+J38+J56+J74</f>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="K90" s="85">
-        <f>K20+K38+K56+K74</f>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="L90" s="85">
-        <f>L20+L38+L56+L74</f>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="M90" s="85">
-        <f>M20+M38+M56+M74</f>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="N90" s="85">
-        <f>N20+N38+N56+N74</f>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="O90" s="86">
-        <f>O20+O38+O56+O74</f>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="P90" s="36">
-        <f t="shared" si="8"/>
-        <v>6966.3255199999994</v>
-      </c>
-    </row>
-    <row r="91" spans="1:16">
+        <f t="shared" si="23"/>
+        <v>10328.265415759022</v>
+      </c>
+    </row>
+    <row r="91" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A91" s="83" t="s">
         <v>37</v>
       </c>
@@ -3968,63 +4606,63 @@
         <v>30</v>
       </c>
       <c r="C91" s="85">
-        <f>C21+C39+C57+C75</f>
-        <v>3417.7370000000001</v>
+        <f t="shared" ref="C91:O91" si="26">C21+C39+C57+C75</f>
+        <v>5155.3427990050513</v>
       </c>
       <c r="D91" s="85">
-        <f>D21+D39+D57+D75</f>
-        <v>2817.9180000000001</v>
+        <f t="shared" si="26"/>
+        <v>4294.7260102158862</v>
       </c>
       <c r="E91" s="85">
-        <f>E21+E39+E57+E75</f>
-        <v>2534.7190000000001</v>
+        <f t="shared" si="26"/>
+        <v>3863.9057938293527</v>
       </c>
       <c r="F91" s="85">
-        <f>F21+F39+F57+F75</f>
-        <v>2281.4229999999998</v>
+        <f t="shared" si="26"/>
+        <v>3477.4472891239757</v>
       </c>
       <c r="G91" s="85">
-        <f>G21+G39+G57+G75</f>
-        <v>2212.9803099999999</v>
+        <f t="shared" si="26"/>
+        <v>3373.1238704502566</v>
       </c>
       <c r="H91" s="85">
-        <f>H21+H39+H57+H75</f>
+        <f t="shared" si="26"/>
         <v>0</v>
       </c>
       <c r="I91" s="85">
-        <f>I21+I39+I57+I75</f>
+        <f t="shared" si="26"/>
         <v>0</v>
       </c>
       <c r="J91" s="85">
-        <f>J21+J39+J57+J75</f>
+        <f t="shared" si="26"/>
         <v>0</v>
       </c>
       <c r="K91" s="85">
-        <f>K21+K39+K57+K75</f>
+        <f t="shared" si="26"/>
         <v>0</v>
       </c>
       <c r="L91" s="85">
-        <f>L21+L39+L57+L75</f>
+        <f t="shared" si="26"/>
         <v>0</v>
       </c>
       <c r="M91" s="85">
-        <f>M21+M39+M57+M75</f>
+        <f t="shared" si="26"/>
         <v>0</v>
       </c>
       <c r="N91" s="85">
-        <f>N21+N39+N57+N75</f>
+        <f t="shared" si="26"/>
         <v>0</v>
       </c>
       <c r="O91" s="86">
-        <f>O21+O39+O57+O75</f>
+        <f t="shared" si="26"/>
         <v>0</v>
       </c>
       <c r="P91" s="36">
-        <f t="shared" si="8"/>
-        <v>13264.777309999998</v>
-      </c>
-    </row>
-    <row r="92" spans="1:16">
+        <f t="shared" si="23"/>
+        <v>20164.545762624522</v>
+      </c>
+    </row>
+    <row r="92" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A92" s="87" t="s">
         <v>39</v>
       </c>
@@ -4032,60 +4670,60 @@
         <v>31</v>
       </c>
       <c r="C92" s="89">
-        <f t="shared" ref="C92:O92" si="9">SUM(C87:C91)</f>
-        <v>16451.8105</v>
+        <f t="shared" ref="C92:O92" si="27">SUM(C87:C91)</f>
+        <v>19680.614222929784</v>
       </c>
       <c r="D92" s="89">
-        <f t="shared" si="9"/>
-        <v>13796.995000000001</v>
+        <f t="shared" si="27"/>
+        <v>16541.107673888218</v>
       </c>
       <c r="E92" s="89">
-        <f t="shared" si="9"/>
-        <v>12414.084500000001</v>
+        <f t="shared" si="27"/>
+        <v>14883.892702414181</v>
       </c>
       <c r="F92" s="89">
-        <f t="shared" si="9"/>
-        <v>11173.34</v>
+        <f t="shared" si="27"/>
+        <v>13395.721865426876</v>
       </c>
       <c r="G92" s="89">
-        <f t="shared" si="9"/>
-        <v>10838.139800000001</v>
+        <f t="shared" si="27"/>
+        <v>12993.850209464068</v>
       </c>
       <c r="H92" s="89">
-        <f t="shared" si="9"/>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="I92" s="89">
-        <f t="shared" si="9"/>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="J92" s="89">
-        <f t="shared" si="9"/>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="K92" s="89">
-        <f t="shared" si="9"/>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="L92" s="89">
-        <f t="shared" si="9"/>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="M92" s="89">
-        <f t="shared" si="9"/>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="N92" s="89">
-        <f t="shared" si="9"/>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="O92" s="90">
-        <f t="shared" si="9"/>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="P92" s="91">
-        <f t="shared" si="8"/>
-        <v>64674.3698</v>
+        <f t="shared" si="23"/>
+        <v>77495.186674123135</v>
       </c>
     </row>
   </sheetData>
@@ -4097,7 +4735,7 @@
     <mergeCell ref="B13:O13"/>
   </mergeCells>
   <pageMargins left="0.75000000000000011" right="0.75000000000000011" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" scale="67" fitToHeight="2" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup paperSize="9" scale="67" fitToHeight="2" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="100"/>

</xml_diff>

<commit_message>
forecasts for jp, sa, nz
</commit_message>
<xml_diff>
--- a/Time Series Analysis/iShades APAC v1.1.xlsx
+++ b/Time Series Analysis/iShades APAC v1.1.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="73">
   <si>
     <t>PRODUCT DEMAND ANALYSIS - iShades</t>
   </si>
@@ -161,29 +161,102 @@
     <t>Question 3:  Zooming in on Japan RSLR, we have 1000 units of each colour in current inventory and we have another 3000 units available (colour yet to be defined), what mix would you build these units ?</t>
   </si>
   <si>
-    <t>Ratio to Pink</t>
-  </si>
-  <si>
-    <t>Ratio to Silver</t>
-  </si>
-  <si>
     <t>Average</t>
   </si>
   <si>
-    <t>Overall Average</t>
+    <t>Red, Green, Blue Ratio to Pink</t>
+  </si>
+  <si>
+    <t>Red, Green, Blue Ratio to Silver</t>
+  </si>
+  <si>
+    <t>Derived Red, Green, Blue Ratio to Silver</t>
+  </si>
+  <si>
+    <t>Derived Red, Green, Blue Ratio to Pink</t>
+  </si>
+  <si>
+    <t>Ratio</t>
+  </si>
+  <si>
+    <t>Average Derived Red, Green, Blue Sales for South Asia</t>
+  </si>
+  <si>
+    <t>Japan 2011</t>
+  </si>
+  <si>
+    <t>New Zealand 2011</t>
+  </si>
+  <si>
+    <t>South Asia 2011</t>
+  </si>
+  <si>
+    <t>Population (1000)</t>
+  </si>
+  <si>
+    <t>South Asia is composed of the following:</t>
+  </si>
+  <si>
+    <t>Afghanistan</t>
+  </si>
+  <si>
+    <t>Bangladesh</t>
+  </si>
+  <si>
+    <t>Bhutan</t>
+  </si>
+  <si>
+    <t>Brunei</t>
+  </si>
+  <si>
+    <t>Cambodia</t>
+  </si>
+  <si>
+    <t>Guam</t>
+  </si>
+  <si>
+    <t> Indonesia</t>
+  </si>
+  <si>
+    <t> Laos</t>
+  </si>
+  <si>
+    <t>Singapore</t>
+  </si>
+  <si>
+    <t>Malaysia</t>
+  </si>
+  <si>
+    <t>Nepal</t>
+  </si>
+  <si>
+    <t>Pakistan</t>
+  </si>
+  <si>
+    <t>Philippines</t>
+  </si>
+  <si>
+    <t>Sri Lanka</t>
+  </si>
+  <si>
+    <t>Vietnam</t>
+  </si>
+  <si>
+    <t>* based on https://www.apple.com/legal/warranty/obligor.html</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="4">
+  <numFmts count="5">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* &quot;-&quot;?_);_(@_)"/>
     <numFmt numFmtId="166" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;?_);_(@_)"/>
+    <numFmt numFmtId="171" formatCode="0.000"/>
   </numFmts>
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -300,6 +373,13 @@
     </font>
     <font>
       <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF333333"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -536,7 +616,7 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="110">
+  <cellXfs count="132">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -677,16 +757,7 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="1" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -701,6 +772,55 @@
     <xf numFmtId="1" fontId="17" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="171" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="171" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="171" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="171" fontId="8" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="171" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="171" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="171" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="171" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="171" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="22">
     <cellStyle name="?" xfId="3"/>
@@ -1064,104 +1184,108 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AB92"/>
+  <dimension ref="A1:AB117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="V58" sqref="V58"/>
+    <sheetView tabSelected="1" topLeftCell="G84" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="120" workbookViewId="0">
+      <selection activeCell="V96" sqref="V96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.125" customWidth="1"/>
     <col min="2" max="2" width="18.875" customWidth="1"/>
-    <col min="3" max="15" width="8.625" customWidth="1"/>
+    <col min="3" max="12" width="8.625" customWidth="1"/>
+    <col min="13" max="13" width="9.5" customWidth="1"/>
+    <col min="14" max="15" width="8.625" customWidth="1"/>
     <col min="16" max="16" width="9" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.125" customWidth="1"/>
+    <col min="18" max="18" width="11" style="116"/>
     <col min="19" max="19" width="12.5" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="13.5" customWidth="1"/>
     <col min="21" max="21" width="12.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="102" t="s">
+    <row r="1" spans="1:21" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="107" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="102"/>
-      <c r="C1" s="102"/>
-      <c r="D1" s="102"/>
-      <c r="E1" s="102"/>
-      <c r="F1" s="102"/>
-      <c r="G1" s="102"/>
-      <c r="H1" s="102"/>
-      <c r="I1" s="102"/>
-      <c r="J1" s="102"/>
-      <c r="K1" s="102"/>
-      <c r="L1" s="102"/>
-      <c r="M1" s="102"/>
-      <c r="N1" s="102"/>
-      <c r="O1" s="102"/>
-      <c r="P1" s="102"/>
-    </row>
-    <row r="2" spans="1:18" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="103"/>
-      <c r="C2" s="103"/>
-      <c r="D2" s="103"/>
-      <c r="E2" s="103"/>
-      <c r="F2" s="103"/>
-      <c r="G2" s="103"/>
-      <c r="H2" s="103"/>
-      <c r="I2" s="103"/>
-      <c r="J2" s="103"/>
-      <c r="K2" s="103"/>
-      <c r="L2" s="103"/>
-      <c r="M2" s="103"/>
-      <c r="N2" s="103"/>
-      <c r="O2" s="103"/>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B1" s="107"/>
+      <c r="C1" s="107"/>
+      <c r="D1" s="107"/>
+      <c r="E1" s="107"/>
+      <c r="F1" s="107"/>
+      <c r="G1" s="107"/>
+      <c r="H1" s="107"/>
+      <c r="I1" s="107"/>
+      <c r="J1" s="107"/>
+      <c r="K1" s="107"/>
+      <c r="L1" s="107"/>
+      <c r="M1" s="107"/>
+      <c r="N1" s="107"/>
+      <c r="O1" s="107"/>
+      <c r="P1" s="107"/>
+    </row>
+    <row r="2" spans="1:21" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="108"/>
+      <c r="C2" s="108"/>
+      <c r="D2" s="108"/>
+      <c r="E2" s="108"/>
+      <c r="F2" s="108"/>
+      <c r="G2" s="108"/>
+      <c r="H2" s="108"/>
+      <c r="I2" s="108"/>
+      <c r="J2" s="108"/>
+      <c r="K2" s="108"/>
+      <c r="L2" s="108"/>
+      <c r="M2" s="108"/>
+      <c r="N2" s="108"/>
+      <c r="O2" s="108"/>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="104" t="s">
+      <c r="B3" s="109" t="s">
         <v>40</v>
       </c>
-      <c r="C3" s="104"/>
-      <c r="D3" s="104"/>
-      <c r="E3" s="104"/>
-      <c r="F3" s="104"/>
-      <c r="G3" s="104"/>
-      <c r="H3" s="104"/>
-      <c r="I3" s="104"/>
-      <c r="J3" s="104"/>
-      <c r="K3" s="104"/>
-      <c r="L3" s="104"/>
-      <c r="M3" s="104"/>
-      <c r="N3" s="104"/>
-      <c r="O3" s="104"/>
+      <c r="C3" s="109"/>
+      <c r="D3" s="109"/>
+      <c r="E3" s="109"/>
+      <c r="F3" s="109"/>
+      <c r="G3" s="109"/>
+      <c r="H3" s="109"/>
+      <c r="I3" s="109"/>
+      <c r="J3" s="109"/>
+      <c r="K3" s="109"/>
+      <c r="L3" s="109"/>
+      <c r="M3" s="109"/>
+      <c r="N3" s="109"/>
+      <c r="O3" s="109"/>
       <c r="P3" s="2"/>
       <c r="Q3" s="2"/>
-      <c r="R3" s="2"/>
-    </row>
-    <row r="4" spans="1:18" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R3" s="117"/>
+    </row>
+    <row r="4" spans="1:21" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
-      <c r="B4" s="105"/>
-      <c r="C4" s="105"/>
-      <c r="D4" s="105"/>
-      <c r="E4" s="105"/>
-      <c r="F4" s="105"/>
-      <c r="G4" s="105"/>
-      <c r="H4" s="105"/>
-      <c r="I4" s="105"/>
-      <c r="J4" s="105"/>
-      <c r="K4" s="105"/>
-      <c r="L4" s="105"/>
-      <c r="M4" s="105"/>
-      <c r="N4" s="105"/>
-      <c r="O4" s="105"/>
+      <c r="B4" s="110"/>
+      <c r="C4" s="110"/>
+      <c r="D4" s="110"/>
+      <c r="E4" s="110"/>
+      <c r="F4" s="110"/>
+      <c r="G4" s="110"/>
+      <c r="H4" s="110"/>
+      <c r="I4" s="110"/>
+      <c r="J4" s="110"/>
+      <c r="K4" s="110"/>
+      <c r="L4" s="110"/>
+      <c r="M4" s="110"/>
+      <c r="N4" s="110"/>
+      <c r="O4" s="110"/>
       <c r="P4" s="2"/>
       <c r="Q4" s="2"/>
-      <c r="R4" s="2"/>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R4" s="117"/>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
@@ -1181,9 +1305,9 @@
       <c r="O5" s="2"/>
       <c r="P5" s="2"/>
       <c r="Q5" s="2"/>
-      <c r="R5" s="2"/>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R5" s="117"/>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>3</v>
       </c>
@@ -1203,9 +1327,9 @@
       <c r="O6" s="2"/>
       <c r="P6" s="2"/>
       <c r="Q6" s="2"/>
-      <c r="R6" s="2"/>
-    </row>
-    <row r="7" spans="1:18" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="R6" s="117"/>
+    </row>
+    <row r="7" spans="1:21" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>41</v>
       </c>
@@ -1225,9 +1349,9 @@
       <c r="O7" s="8"/>
       <c r="P7" s="8"/>
       <c r="Q7" s="8"/>
-      <c r="R7" s="8"/>
-    </row>
-    <row r="8" spans="1:18" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="R7" s="118"/>
+    </row>
+    <row r="8" spans="1:21" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>42</v>
       </c>
@@ -1247,9 +1371,9 @@
       <c r="O8" s="8"/>
       <c r="P8" s="8"/>
       <c r="Q8" s="8"/>
-      <c r="R8" s="8"/>
-    </row>
-    <row r="9" spans="1:18" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="R8" s="118"/>
+    </row>
+    <row r="9" spans="1:21" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>44</v>
       </c>
@@ -1269,9 +1393,9 @@
       <c r="O9" s="8"/>
       <c r="P9" s="8"/>
       <c r="Q9" s="8"/>
-      <c r="R9" s="8"/>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R9" s="118"/>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" s="92" t="s">
         <v>4</v>
       </c>
@@ -1291,9 +1415,9 @@
       <c r="O10" s="2"/>
       <c r="P10" s="2"/>
       <c r="Q10" s="2"/>
-      <c r="R10" s="2"/>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R10" s="117"/>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" s="92" t="s">
         <v>5</v>
       </c>
@@ -1313,9 +1437,9 @@
       <c r="O11" s="2"/>
       <c r="P11" s="2"/>
       <c r="Q11" s="2"/>
-      <c r="R11" s="2"/>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R11" s="117"/>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" s="92" t="s">
         <v>43</v>
       </c>
@@ -1335,29 +1459,29 @@
       <c r="O12" s="2"/>
       <c r="P12" s="2"/>
       <c r="Q12" s="2"/>
-      <c r="R12" s="2"/>
-    </row>
-    <row r="13" spans="1:18" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R12" s="117"/>
+    </row>
+    <row r="13" spans="1:21" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="10"/>
-      <c r="B13" s="105"/>
-      <c r="C13" s="105"/>
-      <c r="D13" s="105"/>
-      <c r="E13" s="105"/>
-      <c r="F13" s="105"/>
-      <c r="G13" s="105"/>
-      <c r="H13" s="105"/>
-      <c r="I13" s="105"/>
-      <c r="J13" s="105"/>
-      <c r="K13" s="105"/>
-      <c r="L13" s="105"/>
-      <c r="M13" s="105"/>
-      <c r="N13" s="105"/>
-      <c r="O13" s="105"/>
+      <c r="B13" s="110"/>
+      <c r="C13" s="110"/>
+      <c r="D13" s="110"/>
+      <c r="E13" s="110"/>
+      <c r="F13" s="110"/>
+      <c r="G13" s="110"/>
+      <c r="H13" s="110"/>
+      <c r="I13" s="110"/>
+      <c r="J13" s="110"/>
+      <c r="K13" s="110"/>
+      <c r="L13" s="110"/>
+      <c r="M13" s="110"/>
+      <c r="N13" s="110"/>
+      <c r="O13" s="110"/>
       <c r="P13" s="2"/>
       <c r="Q13" s="2"/>
-      <c r="R13" s="2"/>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="R13" s="117"/>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" s="11"/>
       <c r="D14" s="12"/>
       <c r="E14" s="12"/>
@@ -1369,7 +1493,7 @@
       <c r="L14" s="12"/>
       <c r="N14" s="12"/>
     </row>
-    <row r="15" spans="1:18" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:21" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="13" t="s">
         <v>6</v>
       </c>
@@ -1416,8 +1540,9 @@
         <v>8</v>
       </c>
       <c r="P15"/>
-    </row>
-    <row r="16" spans="1:18" s="21" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="R15" s="119"/>
+    </row>
+    <row r="16" spans="1:21" s="21" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A16" s="17" t="s">
         <v>9</v>
       </c>
@@ -1466,9 +1591,13 @@
       <c r="P16" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="Q16" s="21" t="s">
-        <v>46</v>
-      </c>
+      <c r="Q16" s="112" t="s">
+        <v>47</v>
+      </c>
+      <c r="R16" s="111"/>
+      <c r="S16" s="111"/>
+      <c r="T16" s="111"/>
+      <c r="U16" s="111"/>
     </row>
     <row r="17" spans="1:26" s="30" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="22" t="s">
@@ -1492,18 +1621,35 @@
       <c r="G17" s="24">
         <v>1592.74</v>
       </c>
-      <c r="H17" s="25"/>
-      <c r="I17" s="25"/>
-      <c r="J17" s="25"/>
-      <c r="K17" s="25"/>
-      <c r="L17" s="25"/>
-      <c r="M17" s="25"/>
-      <c r="N17" s="25"/>
-      <c r="O17" s="26"/>
+      <c r="H17" s="25">
+        <v>2681.9259999999999</v>
+      </c>
+      <c r="I17" s="25">
+        <v>2340.3609999999999</v>
+      </c>
+      <c r="J17" s="25">
+        <v>2132.7350000000001</v>
+      </c>
+      <c r="K17" s="25">
+        <v>2006.5260000000001</v>
+      </c>
+      <c r="L17" s="25">
+        <v>1929.808</v>
+      </c>
+      <c r="M17" s="25">
+        <v>1883.174</v>
+      </c>
+      <c r="N17" s="25">
+        <v>1854.826</v>
+      </c>
+      <c r="O17" s="26">
+        <v>1837.595</v>
+      </c>
       <c r="P17" s="27">
         <f>SUM(C17:O17)</f>
-        <v>9479.74</v>
-      </c>
+        <v>26146.691000000003</v>
+      </c>
+      <c r="R17" s="120"/>
       <c r="S17" s="29"/>
       <c r="T17" s="29"/>
       <c r="U17" s="29"/>
@@ -1536,35 +1682,51 @@
       <c r="G18" s="33">
         <v>1101.92</v>
       </c>
-      <c r="H18" s="34"/>
-      <c r="I18" s="34"/>
-      <c r="J18" s="34"/>
-      <c r="K18" s="34"/>
-      <c r="L18" s="34"/>
-      <c r="M18" s="34"/>
-      <c r="N18" s="34"/>
-      <c r="O18" s="35"/>
+      <c r="H18" s="34">
+        <v>1843.0820000000001</v>
+      </c>
+      <c r="I18" s="34">
+        <v>1611.307</v>
+      </c>
+      <c r="J18" s="34">
+        <v>1470.4179999999999</v>
+      </c>
+      <c r="K18" s="34">
+        <v>1384.777</v>
+      </c>
+      <c r="L18" s="34">
+        <v>1332.7180000000001</v>
+      </c>
+      <c r="M18" s="34">
+        <v>1301.0730000000001</v>
+      </c>
+      <c r="N18" s="34">
+        <v>1281.838</v>
+      </c>
+      <c r="O18" s="35">
+        <v>1270.145</v>
+      </c>
       <c r="P18" s="36">
         <f t="shared" ref="P18:P22" si="0">SUM(C18:O18)</f>
-        <v>6548.92</v>
-      </c>
-      <c r="Q18" s="106">
+        <v>18044.278000000002</v>
+      </c>
+      <c r="Q18" s="103">
         <v>1</v>
       </c>
-      <c r="R18" s="106">
+      <c r="R18" s="121">
         <v>2</v>
       </c>
-      <c r="S18" s="106">
+      <c r="S18" s="103">
         <v>3</v>
       </c>
-      <c r="T18" s="106">
+      <c r="T18" s="103">
         <v>4</v>
       </c>
-      <c r="U18" s="106">
+      <c r="U18" s="103">
         <v>5</v>
       </c>
       <c r="V18" s="29" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="19" spans="1:26" s="30" customFormat="1" x14ac:dyDescent="0.25">
@@ -1590,23 +1752,39 @@
       <c r="G19" s="33">
         <v>445.22999999999996</v>
       </c>
-      <c r="H19" s="34"/>
-      <c r="I19" s="34"/>
-      <c r="J19" s="34"/>
-      <c r="K19" s="34"/>
-      <c r="L19" s="34"/>
-      <c r="M19" s="34"/>
-      <c r="N19" s="34"/>
-      <c r="O19" s="35"/>
+      <c r="H19" s="34">
+        <v>761.13199999999995</v>
+      </c>
+      <c r="I19" s="34">
+        <v>661.55700000000002</v>
+      </c>
+      <c r="J19" s="34">
+        <v>601.029</v>
+      </c>
+      <c r="K19" s="34">
+        <v>564.23699999999997</v>
+      </c>
+      <c r="L19" s="34">
+        <v>541.87099999999998</v>
+      </c>
+      <c r="M19" s="34">
+        <v>528.27599999999995</v>
+      </c>
+      <c r="N19" s="34">
+        <v>520.01199999999994</v>
+      </c>
+      <c r="O19" s="35">
+        <v>514.98900000000003</v>
+      </c>
       <c r="P19" s="36">
         <f t="shared" si="0"/>
-        <v>2660.23</v>
+        <v>7353.3330000000005</v>
       </c>
       <c r="Q19" s="28">
         <f>C19/C$17</f>
         <v>0.28362573099415206</v>
       </c>
-      <c r="R19" s="28">
+      <c r="R19" s="122">
         <f t="shared" ref="R19:U21" si="1">D19/D$17</f>
         <v>0.27972372964972864</v>
       </c>
@@ -1650,23 +1828,39 @@
       <c r="G20" s="33">
         <v>818.68</v>
       </c>
-      <c r="H20" s="34"/>
-      <c r="I20" s="34"/>
-      <c r="J20" s="34"/>
-      <c r="K20" s="34"/>
-      <c r="L20" s="34"/>
-      <c r="M20" s="34"/>
-      <c r="N20" s="34"/>
-      <c r="O20" s="35"/>
+      <c r="H20" s="34">
+        <v>1441.3109999999999</v>
+      </c>
+      <c r="I20" s="34">
+        <v>1243.211</v>
+      </c>
+      <c r="J20" s="34">
+        <v>1122.7929999999999</v>
+      </c>
+      <c r="K20" s="34">
+        <v>1049.595</v>
+      </c>
+      <c r="L20" s="34">
+        <v>1005.1</v>
+      </c>
+      <c r="M20" s="34">
+        <v>978.053</v>
+      </c>
+      <c r="N20" s="34">
+        <v>961.61199999999997</v>
+      </c>
+      <c r="O20" s="35">
+        <v>951.61800000000005</v>
+      </c>
       <c r="P20" s="36">
         <f t="shared" si="0"/>
-        <v>4926.68</v>
+        <v>13679.973</v>
       </c>
       <c r="Q20" s="28">
         <f t="shared" ref="Q20:Q21" si="2">C20/C$17</f>
         <v>0.53675856307435255</v>
       </c>
-      <c r="R20" s="28">
+      <c r="R20" s="122">
         <f t="shared" si="1"/>
         <v>0.51406018746916626</v>
       </c>
@@ -1683,7 +1877,7 @@
         <v>0.51400730816077955</v>
       </c>
       <c r="V20" s="28">
-        <f t="shared" ref="V20:V30" si="3">AVERAGE(Q20:U20)</f>
+        <f t="shared" ref="V20:V21" si="3">AVERAGE(Q20:U20)</f>
         <v>0.51850790144319103</v>
       </c>
     </row>
@@ -1710,23 +1904,39 @@
       <c r="G21" s="33">
         <v>1258.0899999999999</v>
       </c>
-      <c r="H21" s="34"/>
-      <c r="I21" s="34"/>
-      <c r="J21" s="34"/>
-      <c r="K21" s="34"/>
-      <c r="L21" s="34"/>
-      <c r="M21" s="34"/>
-      <c r="N21" s="34"/>
-      <c r="O21" s="35"/>
+      <c r="H21" s="34">
+        <v>2178.5239999999999</v>
+      </c>
+      <c r="I21" s="34">
+        <v>1887.2370000000001</v>
+      </c>
+      <c r="J21" s="34">
+        <v>1710.174</v>
+      </c>
+      <c r="K21" s="34">
+        <v>1602.5429999999999</v>
+      </c>
+      <c r="L21" s="34">
+        <v>1537.1179999999999</v>
+      </c>
+      <c r="M21" s="34">
+        <v>1497.348</v>
+      </c>
+      <c r="N21" s="34">
+        <v>1473.173</v>
+      </c>
+      <c r="O21" s="35">
+        <v>1458.4780000000001</v>
+      </c>
       <c r="P21" s="36">
         <f t="shared" si="0"/>
-        <v>7541.09</v>
+        <v>20885.684999999998</v>
       </c>
       <c r="Q21" s="28">
         <f t="shared" si="2"/>
         <v>0.81161236424394323</v>
       </c>
-      <c r="R21" s="28">
+      <c r="R21" s="122">
         <f t="shared" si="1"/>
         <v>0.79033053774050321</v>
       </c>
@@ -1777,51 +1987,52 @@
       </c>
       <c r="H22" s="39">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>8905.9749999999985</v>
       </c>
       <c r="I22" s="39">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>7743.6729999999998</v>
       </c>
       <c r="J22" s="39">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>7037.1490000000003</v>
       </c>
       <c r="K22" s="39">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>6607.6779999999999</v>
       </c>
       <c r="L22" s="39">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>6346.6149999999998</v>
       </c>
       <c r="M22" s="39">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>6187.924</v>
       </c>
       <c r="N22" s="39">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>6091.4609999999993</v>
       </c>
       <c r="O22" s="40">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>6032.8249999999998</v>
       </c>
       <c r="P22" s="41">
         <f t="shared" si="0"/>
-        <v>31156.66</v>
-      </c>
+        <v>86109.959999999992</v>
+      </c>
+      <c r="R22" s="123"/>
       <c r="V22" s="28"/>
     </row>
     <row r="23" spans="1:26" s="96" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="93"/>
       <c r="B23" s="94"/>
       <c r="C23" s="97"/>
-      <c r="D23" s="97"/>
-      <c r="E23" s="97"/>
-      <c r="F23" s="97"/>
-      <c r="G23" s="97"/>
-      <c r="H23" s="97"/>
+      <c r="D23" s="114"/>
+      <c r="E23" s="114"/>
+      <c r="F23" s="114"/>
+      <c r="G23" s="114"/>
+      <c r="H23" s="114"/>
       <c r="I23" s="97"/>
       <c r="J23" s="97"/>
       <c r="K23" s="97"/>
@@ -1830,6 +2041,7 @@
       <c r="N23" s="97"/>
       <c r="O23" s="98"/>
       <c r="P23" s="95"/>
+      <c r="R23" s="124"/>
       <c r="V23" s="28"/>
     </row>
     <row r="24" spans="1:26" s="96" customFormat="1" x14ac:dyDescent="0.25">
@@ -1875,6 +2087,7 @@
         <v>7</v>
       </c>
       <c r="P24" s="95"/>
+      <c r="R24" s="124"/>
       <c r="V24" s="28"/>
     </row>
     <row r="25" spans="1:26" ht="31.5" x14ac:dyDescent="0.25">
@@ -1922,9 +2135,13 @@
         <v>23</v>
       </c>
       <c r="P25" s="45"/>
-      <c r="Q25" s="21" t="s">
-        <v>45</v>
-      </c>
+      <c r="Q25" s="112" t="s">
+        <v>46</v>
+      </c>
+      <c r="R25" s="111"/>
+      <c r="S25" s="111"/>
+      <c r="T25" s="111"/>
+      <c r="U25" s="111"/>
       <c r="V25" s="28"/>
     </row>
     <row r="26" spans="1:26" s="51" customFormat="1" x14ac:dyDescent="0.25">
@@ -1977,6 +2194,7 @@
         <f>SUM(C26:O26)</f>
         <v>101087.70107538856</v>
       </c>
+      <c r="R26" s="125"/>
     </row>
     <row r="27" spans="1:26" s="57" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="52" t="s">
@@ -1997,23 +2215,23 @@
       <c r="N27" s="54"/>
       <c r="O27" s="55"/>
       <c r="P27" s="56"/>
-      <c r="Q27" s="107">
+      <c r="Q27" s="104">
         <v>1</v>
       </c>
-      <c r="R27" s="108">
+      <c r="R27" s="126">
         <v>2</v>
       </c>
-      <c r="S27" s="108">
+      <c r="S27" s="105">
         <v>3</v>
       </c>
-      <c r="T27" s="108">
+      <c r="T27" s="105">
         <v>4</v>
       </c>
-      <c r="U27" s="108">
+      <c r="U27" s="105">
         <v>5</v>
       </c>
-      <c r="V27" s="109" t="s">
-        <v>47</v>
+      <c r="V27" s="106" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="28" spans="1:26" s="57" customFormat="1" x14ac:dyDescent="0.25">
@@ -2034,23 +2252,23 @@
       <c r="O28" s="59"/>
       <c r="P28" s="60"/>
       <c r="Q28" s="28">
-        <f>C19/C$18</f>
+        <f t="shared" ref="Q28:U30" si="5">C19/C$18</f>
         <v>0.4127659574468085</v>
       </c>
-      <c r="R28" s="28">
-        <f>D19/D$18</f>
+      <c r="R28" s="122">
+        <f t="shared" si="5"/>
         <v>0.40413399857448323</v>
       </c>
       <c r="S28" s="28">
-        <f>E19/E$18</f>
+        <f t="shared" si="5"/>
         <v>0.40380047505938244</v>
       </c>
       <c r="T28" s="28">
-        <f>F19/F$18</f>
+        <f t="shared" si="5"/>
         <v>0.40404929577464788</v>
       </c>
       <c r="U28" s="28">
-        <f>G19/G$18</f>
+        <f t="shared" si="5"/>
         <v>0.40404929577464782</v>
       </c>
       <c r="V28" s="28">
@@ -2076,23 +2294,23 @@
       <c r="O29" s="62"/>
       <c r="P29" s="63"/>
       <c r="Q29" s="28">
-        <f>C20/C$18</f>
+        <f t="shared" si="5"/>
         <v>0.78115501519756836</v>
       </c>
-      <c r="R29" s="28">
-        <f>D20/D$18</f>
+      <c r="R29" s="122">
+        <f t="shared" si="5"/>
         <v>0.74269422665716323</v>
       </c>
       <c r="S29" s="28">
-        <f>E20/E$18</f>
+        <f t="shared" si="5"/>
         <v>0.74188440221694374</v>
       </c>
       <c r="T29" s="28">
-        <f>F20/F$18</f>
+        <f t="shared" si="5"/>
         <v>0.74295774647887325</v>
       </c>
       <c r="U29" s="28">
-        <f>G20/G$18</f>
+        <f t="shared" si="5"/>
         <v>0.74295774647887314</v>
       </c>
       <c r="V29" s="28">
@@ -2118,23 +2336,23 @@
       <c r="O30" s="62"/>
       <c r="P30" s="63"/>
       <c r="Q30" s="28">
-        <f>C21/C$18</f>
+        <f t="shared" si="5"/>
         <v>1.1811550151975685</v>
       </c>
-      <c r="R30" s="28">
-        <f>D21/D$18</f>
+      <c r="R30" s="122">
+        <f t="shared" si="5"/>
         <v>1.1418389166072702</v>
       </c>
       <c r="S30" s="28">
-        <f>E21/E$18</f>
+        <f t="shared" si="5"/>
         <v>1.1409342834520981</v>
       </c>
       <c r="T30" s="28">
-        <f>F21/F$18</f>
+        <f t="shared" si="5"/>
         <v>1.141725352112676</v>
       </c>
       <c r="U30" s="28">
-        <f>G21/G$18</f>
+        <f t="shared" si="5"/>
         <v>1.141725352112676</v>
       </c>
       <c r="V30" s="28">
@@ -2159,6 +2377,7 @@
       <c r="N31" s="66"/>
       <c r="O31" s="67"/>
       <c r="P31" s="68"/>
+      <c r="R31" s="127"/>
     </row>
     <row r="32" spans="1:26" x14ac:dyDescent="0.25">
       <c r="C32" s="12"/>
@@ -2218,6 +2437,7 @@
         <v>8</v>
       </c>
       <c r="P33"/>
+      <c r="R33" s="119"/>
     </row>
     <row r="34" spans="1:28" s="21" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A34" s="17" t="s">
@@ -2268,9 +2488,13 @@
       <c r="P34" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="Q34" s="21" t="s">
-        <v>46</v>
-      </c>
+      <c r="Q34" s="112" t="s">
+        <v>48</v>
+      </c>
+      <c r="R34" s="111"/>
+      <c r="S34" s="111"/>
+      <c r="T34" s="111"/>
+      <c r="U34" s="111"/>
     </row>
     <row r="35" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A35" s="69" t="s">
@@ -2294,19 +2518,35 @@
       <c r="G35" s="70">
         <v>1400.81483</v>
       </c>
-      <c r="H35" s="25"/>
-      <c r="I35" s="25"/>
-      <c r="J35" s="25"/>
-      <c r="K35" s="25"/>
-      <c r="L35" s="25"/>
-      <c r="M35" s="25"/>
-      <c r="N35" s="25"/>
-      <c r="O35" s="26"/>
+      <c r="H35" s="25">
+        <v>2034.393</v>
+      </c>
+      <c r="I35" s="25">
+        <v>2319.0569999999998</v>
+      </c>
+      <c r="J35" s="25">
+        <v>1981.2840000000001</v>
+      </c>
+      <c r="K35" s="25">
+        <v>1796.07</v>
+      </c>
+      <c r="L35" s="25">
+        <v>1694.51</v>
+      </c>
+      <c r="M35" s="25">
+        <v>1638.8209999999999</v>
+      </c>
+      <c r="N35" s="25">
+        <v>1608.2840000000001</v>
+      </c>
+      <c r="O35" s="26">
+        <v>1591.54</v>
+      </c>
       <c r="P35" s="27">
         <f>SUM(C35:O35)</f>
-        <v>8337.4313299999994</v>
-      </c>
-      <c r="R35" s="71"/>
+        <v>23001.390329999998</v>
+      </c>
+      <c r="R35" s="120"/>
       <c r="S35" s="71"/>
       <c r="T35" s="71"/>
       <c r="U35" s="71"/>
@@ -2335,23 +2575,53 @@
       <c r="G36" s="72">
         <v>817.07367999999997</v>
       </c>
-      <c r="H36" s="34"/>
-      <c r="I36" s="34"/>
-      <c r="J36" s="34"/>
-      <c r="K36" s="34"/>
-      <c r="L36" s="34"/>
-      <c r="M36" s="34"/>
-      <c r="N36" s="34"/>
-      <c r="O36" s="35"/>
+      <c r="H36" s="34">
+        <v>1180.998</v>
+      </c>
+      <c r="I36" s="34">
+        <v>1343.9459999999999</v>
+      </c>
+      <c r="J36" s="34">
+        <v>1150.6780000000001</v>
+      </c>
+      <c r="K36" s="34">
+        <v>1044.701</v>
+      </c>
+      <c r="L36" s="34">
+        <v>986.59</v>
+      </c>
+      <c r="M36" s="34">
+        <v>954.726</v>
+      </c>
+      <c r="N36" s="34">
+        <v>937.25300000000004</v>
+      </c>
+      <c r="O36" s="35">
+        <v>927.67200000000003</v>
+      </c>
       <c r="P36" s="36">
-        <f t="shared" ref="P36:P39" si="5">SUM(C36:O36)</f>
-        <v>4856.0241800000003</v>
-      </c>
-      <c r="R36" s="71"/>
-      <c r="S36" s="71"/>
-      <c r="T36" s="71"/>
-      <c r="U36" s="71"/>
-      <c r="V36" s="71"/>
+        <f t="shared" ref="P36:P39" si="6">SUM(C36:O36)</f>
+        <v>13382.588180000002</v>
+      </c>
+      <c r="Q36" s="102" t="s">
+        <v>50</v>
+      </c>
+      <c r="R36" s="119">
+        <v>1</v>
+      </c>
+      <c r="S36" s="102">
+        <v>2</v>
+      </c>
+      <c r="T36" s="102">
+        <v>3</v>
+      </c>
+      <c r="U36" s="102">
+        <v>4</v>
+      </c>
+      <c r="V36" s="102">
+        <v>5</v>
+      </c>
+      <c r="W36" s="113"/>
     </row>
     <row r="37" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A37" s="31" t="str">
@@ -2376,23 +2646,39 @@
       <c r="G37" s="72">
         <v>430.29612466108676</v>
       </c>
-      <c r="H37" s="34"/>
-      <c r="I37" s="34"/>
-      <c r="J37" s="34"/>
-      <c r="K37" s="34"/>
-      <c r="L37" s="34"/>
-      <c r="M37" s="34"/>
-      <c r="N37" s="34"/>
-      <c r="O37" s="35"/>
+      <c r="H37" s="34">
+        <v>623.03399999999999</v>
+      </c>
+      <c r="I37" s="34">
+        <v>709.41</v>
+      </c>
+      <c r="J37" s="34">
+        <v>606.95000000000005</v>
+      </c>
+      <c r="K37" s="34">
+        <v>550.76700000000005</v>
+      </c>
+      <c r="L37" s="34">
+        <v>519.96</v>
+      </c>
+      <c r="M37" s="34">
+        <v>503.06700000000001</v>
+      </c>
+      <c r="N37" s="34">
+        <v>493.80399999999997</v>
+      </c>
+      <c r="O37" s="35">
+        <v>488.72500000000002</v>
+      </c>
       <c r="P37" s="36">
-        <f t="shared" si="5"/>
-        <v>2559.1085257395839</v>
+        <f t="shared" si="6"/>
+        <v>7054.825525739584</v>
       </c>
       <c r="Q37" s="64">
         <f>AVERAGE(V19,V55)</f>
         <v>0.29315152308214953</v>
       </c>
-      <c r="R37" s="29">
+      <c r="R37" s="120">
         <f>$Q37*C$35</f>
         <v>617.23727433449676</v>
       </c>
@@ -2409,7 +2695,7 @@
         <v>423.35154739233241</v>
       </c>
       <c r="V37" s="29">
-        <f t="shared" ref="S37:V39" si="6">$Q37*G$35</f>
+        <f t="shared" ref="S37:V39" si="7">$Q37*G$35</f>
         <v>410.65100097056239</v>
       </c>
     </row>
@@ -2436,32 +2722,48 @@
       <c r="G38" s="72">
         <v>565.27072435272657</v>
       </c>
-      <c r="H38" s="34"/>
-      <c r="I38" s="34"/>
-      <c r="J38" s="34"/>
-      <c r="K38" s="34"/>
-      <c r="L38" s="34"/>
-      <c r="M38" s="34"/>
-      <c r="N38" s="34"/>
-      <c r="O38" s="35"/>
+      <c r="H38" s="34">
+        <v>819.23400000000004</v>
+      </c>
+      <c r="I38" s="34">
+        <v>933.09100000000001</v>
+      </c>
+      <c r="J38" s="34">
+        <v>798.02700000000004</v>
+      </c>
+      <c r="K38" s="34">
+        <v>723.96699999999998</v>
+      </c>
+      <c r="L38" s="34">
+        <v>683.35699999999997</v>
+      </c>
+      <c r="M38" s="34">
+        <v>661.08900000000006</v>
+      </c>
+      <c r="N38" s="34">
+        <v>648.87850000000003</v>
+      </c>
+      <c r="O38" s="35">
+        <v>642.18299999999999</v>
+      </c>
       <c r="P38" s="36">
-        <f t="shared" si="5"/>
-        <v>3361.9398957590233</v>
+        <f t="shared" si="6"/>
+        <v>9271.766395759023</v>
       </c>
       <c r="Q38" s="64">
         <f>AVERAGE(V20,V56)</f>
         <v>0.40066519656973848</v>
       </c>
-      <c r="R38" s="29">
+      <c r="R38" s="120">
         <f>$Q38*C$35</f>
         <v>843.60978667710549</v>
       </c>
       <c r="S38" s="29">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>714.28447685651315</v>
       </c>
       <c r="T38" s="29">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>642.75031365874702</v>
       </c>
       <c r="U38" s="29">
@@ -2469,7 +2771,7 @@
         <v>578.61623630902557</v>
       </c>
       <c r="V38" s="29">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>561.25774921975483</v>
       </c>
     </row>
@@ -2496,23 +2798,39 @@
       <c r="G39" s="72">
         <v>1160.1435604502567</v>
       </c>
-      <c r="H39" s="34"/>
-      <c r="I39" s="34"/>
-      <c r="J39" s="34"/>
-      <c r="K39" s="34"/>
-      <c r="L39" s="34"/>
-      <c r="M39" s="34"/>
-      <c r="N39" s="34"/>
-      <c r="O39" s="35"/>
+      <c r="H39" s="34">
+        <v>1680.77</v>
+      </c>
+      <c r="I39" s="34">
+        <v>1914.289</v>
+      </c>
+      <c r="J39" s="34">
+        <v>1637.2639999999999</v>
+      </c>
+      <c r="K39" s="34">
+        <v>1485.36</v>
+      </c>
+      <c r="L39" s="34">
+        <v>1402.0650000000001</v>
+      </c>
+      <c r="M39" s="34">
+        <v>1356.3910000000001</v>
+      </c>
+      <c r="N39" s="34">
+        <v>1331.346</v>
+      </c>
+      <c r="O39" s="35">
+        <v>1317.6130000000001</v>
+      </c>
       <c r="P39" s="36">
-        <f t="shared" si="5"/>
-        <v>6899.768452624523</v>
+        <f t="shared" si="6"/>
+        <v>19024.866452624527</v>
       </c>
       <c r="Q39" s="64">
         <f>AVERAGE(V21,V57)</f>
         <v>0.79434911739712444</v>
       </c>
-      <c r="R39" s="29">
+      <c r="R39" s="120">
         <f>$Q39*C$35</f>
         <v>1672.5203367093457</v>
       </c>
@@ -2521,11 +2839,11 @@
         <v>1416.1231088178124</v>
       </c>
       <c r="T39" s="29">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1274.3012089214062</v>
       </c>
       <c r="U39" s="29">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1147.1505400487661</v>
       </c>
       <c r="V39" s="29">
@@ -2542,61 +2860,62 @@
         <v>31</v>
       </c>
       <c r="C40" s="39">
-        <f t="shared" ref="C40:O40" si="7">SUM(C35:C39)</f>
+        <f t="shared" ref="C40:O40" si="8">SUM(C35:C39)</f>
         <v>6554.0942229297834</v>
       </c>
       <c r="D40" s="39">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>5567.1836738882175</v>
       </c>
       <c r="E40" s="39">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>5010.530702414183</v>
       </c>
       <c r="F40" s="39">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>4508.8648654268763</v>
       </c>
       <c r="G40" s="39">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>4373.5989194640697</v>
       </c>
       <c r="H40" s="39">
-        <f t="shared" si="7"/>
-        <v>0</v>
+        <f>SUM(H35:H39)</f>
+        <v>6338.4290000000001</v>
       </c>
       <c r="I40" s="39">
-        <f t="shared" si="7"/>
-        <v>0</v>
+        <f t="shared" si="8"/>
+        <v>7219.7929999999997</v>
       </c>
       <c r="J40" s="39">
-        <f t="shared" si="7"/>
-        <v>0</v>
+        <f t="shared" si="8"/>
+        <v>6174.2030000000004</v>
       </c>
       <c r="K40" s="39">
-        <f t="shared" si="7"/>
-        <v>0</v>
+        <f t="shared" si="8"/>
+        <v>5600.8649999999989</v>
       </c>
       <c r="L40" s="39">
-        <f t="shared" si="7"/>
-        <v>0</v>
+        <f t="shared" si="8"/>
+        <v>5286.482</v>
       </c>
       <c r="M40" s="39">
-        <f t="shared" si="7"/>
-        <v>0</v>
+        <f t="shared" si="8"/>
+        <v>5114.0940000000001</v>
       </c>
       <c r="N40" s="39">
-        <f t="shared" si="7"/>
-        <v>0</v>
+        <f t="shared" si="8"/>
+        <v>5019.5655000000006</v>
       </c>
       <c r="O40" s="40">
-        <f t="shared" si="7"/>
-        <v>0</v>
+        <f t="shared" si="8"/>
+        <v>4967.7330000000002</v>
       </c>
       <c r="P40" s="41">
         <f>SUM(C40:O40)</f>
-        <v>26014.272384123127</v>
-      </c>
+        <v>71735.436884123133</v>
+      </c>
+      <c r="R40" s="123"/>
     </row>
     <row r="41" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A41" s="43"/>
@@ -2659,6 +2978,7 @@
         <v>7</v>
       </c>
       <c r="P42" s="95"/>
+      <c r="R42" s="124"/>
     </row>
     <row r="43" spans="1:28" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A43" s="43"/>
@@ -2705,12 +3025,20 @@
         <v>23</v>
       </c>
       <c r="P43" s="45"/>
-      <c r="Q43" s="21" t="s">
-        <v>45</v>
-      </c>
-      <c r="X43" t="s">
-        <v>48</v>
-      </c>
+      <c r="Q43" s="112" t="s">
+        <v>49</v>
+      </c>
+      <c r="R43" s="111"/>
+      <c r="S43" s="111"/>
+      <c r="T43" s="111"/>
+      <c r="U43" s="111"/>
+      <c r="X43" s="108" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y43" s="108"/>
+      <c r="Z43" s="108"/>
+      <c r="AA43" s="108"/>
+      <c r="AB43" s="108"/>
     </row>
     <row r="44" spans="1:28" s="51" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="46" t="s">
@@ -2762,6 +3090,7 @@
         <f>SUM(C44:O44)</f>
         <v>43392.412699490647</v>
       </c>
+      <c r="R44" s="125"/>
     </row>
     <row r="45" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A45" s="73" t="s">
@@ -2782,6 +3111,25 @@
       <c r="N45" s="54"/>
       <c r="O45" s="55"/>
       <c r="P45" s="56"/>
+      <c r="Q45" s="102" t="s">
+        <v>50</v>
+      </c>
+      <c r="R45" s="119">
+        <v>1</v>
+      </c>
+      <c r="S45" s="102">
+        <v>2</v>
+      </c>
+      <c r="T45" s="102">
+        <v>3</v>
+      </c>
+      <c r="U45" s="102">
+        <v>4</v>
+      </c>
+      <c r="V45" s="102">
+        <v>5</v>
+      </c>
+      <c r="W45" s="102"/>
       <c r="X45">
         <v>1</v>
       </c>
@@ -2819,24 +3167,24 @@
         <f>AVERAGE(V28,V64)</f>
         <v>0.55067402042813474</v>
       </c>
-      <c r="R46" s="29">
+      <c r="R46" s="120">
         <f>$Q46*C$36</f>
         <v>671.69427321257479</v>
       </c>
       <c r="S46" s="29">
-        <f t="shared" ref="S46:V48" si="8">$Q46*D$36</f>
+        <f t="shared" ref="S46:V48" si="9">$Q46*D$36</f>
         <v>572.87967496488898</v>
       </c>
       <c r="T46" s="29">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>515.71420490424441</v>
       </c>
       <c r="U46" s="29">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>463.85695706351669</v>
       </c>
       <c r="V46" s="29">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>449.94124835161119</v>
       </c>
       <c r="X46" s="57">
@@ -2844,19 +3192,19 @@
         <v>644.46577377353583</v>
       </c>
       <c r="Y46" s="57">
-        <f t="shared" ref="Y46:AB48" si="9">AVERAGE(S37, S46)</f>
+        <f t="shared" ref="Y46:AB48" si="10">AVERAGE(S37, S46)</f>
         <v>547.74726335463015</v>
       </c>
       <c r="Z46" s="57">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>492.9951117224067</v>
       </c>
       <c r="AA46" s="57">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>443.60425222792458</v>
       </c>
       <c r="AB46" s="57">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>430.29612466108676</v>
       </c>
     </row>
@@ -2878,47 +3226,47 @@
       <c r="O47" s="62"/>
       <c r="P47" s="63"/>
       <c r="Q47" s="64">
-        <f t="shared" ref="Q47:Q48" si="10">AVERAGE(V29,V65)</f>
+        <f t="shared" ref="Q47:Q48" si="11">AVERAGE(V29,V65)</f>
         <v>0.69673483973403538</v>
       </c>
-      <c r="R47" s="29">
+      <c r="R47" s="120">
         <f>$Q47*C$36</f>
         <v>849.85451362528499</v>
       </c>
       <c r="S47" s="29">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>724.83032377889049</v>
       </c>
       <c r="T47" s="29">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>652.5022800661003</v>
       </c>
       <c r="U47" s="29">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>586.89041184092628</v>
       </c>
       <c r="V47" s="29">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>569.28369948569843</v>
       </c>
       <c r="X47" s="57">
-        <f t="shared" ref="X47:X48" si="11">AVERAGE(R38, R47)</f>
+        <f t="shared" ref="X47:X48" si="12">AVERAGE(R38, R47)</f>
         <v>846.73215015119524</v>
       </c>
       <c r="Y47" s="57">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>719.55740031770188</v>
       </c>
       <c r="Z47" s="57">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>647.62629686242371</v>
       </c>
       <c r="AA47" s="57">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>582.75332407497592</v>
       </c>
       <c r="AB47" s="57">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>565.27072435272657</v>
       </c>
     </row>
@@ -2940,47 +3288,47 @@
       <c r="O48" s="62"/>
       <c r="P48" s="63"/>
       <c r="Q48" s="64">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>1.4778974364383031</v>
       </c>
-      <c r="R48" s="29">
+      <c r="R48" s="120">
         <f>$Q48*C$36</f>
         <v>1802.6912613007578</v>
       </c>
       <c r="S48" s="29">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1537.4929116139594</v>
       </c>
       <c r="T48" s="29">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1384.0723787372992</v>
       </c>
       <c r="U48" s="29">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1244.898038199186</v>
       </c>
       <c r="V48" s="29">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>1207.5510970532102</v>
       </c>
       <c r="X48" s="57">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1737.6057990050517</v>
       </c>
       <c r="Y48" s="57">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1476.808010215886</v>
       </c>
       <c r="Z48" s="57">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1329.1867938293526</v>
       </c>
       <c r="AA48" s="57">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1196.0242891239759</v>
       </c>
       <c r="AB48" s="57">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>1160.1435604502567</v>
       </c>
     </row>
@@ -3001,6 +3349,7 @@
       <c r="N49" s="66"/>
       <c r="O49" s="67"/>
       <c r="P49" s="68"/>
+      <c r="R49" s="127"/>
     </row>
     <row r="50" spans="1:22" x14ac:dyDescent="0.25">
       <c r="C50" s="12"/>
@@ -3060,6 +3409,7 @@
         <v>8</v>
       </c>
       <c r="P51"/>
+      <c r="R51" s="119"/>
     </row>
     <row r="52" spans="1:22" s="21" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A52" s="17" t="s">
@@ -3110,9 +3460,13 @@
       <c r="P52" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="Q52" s="21" t="s">
-        <v>46</v>
-      </c>
+      <c r="Q52" s="112" t="s">
+        <v>47</v>
+      </c>
+      <c r="R52" s="111"/>
+      <c r="S52" s="111"/>
+      <c r="T52" s="111"/>
+      <c r="U52" s="111"/>
     </row>
     <row r="53" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A53" s="69" t="s">
@@ -3136,20 +3490,36 @@
       <c r="G53" s="70">
         <v>1208.88966</v>
       </c>
-      <c r="H53" s="25"/>
-      <c r="I53" s="25"/>
-      <c r="J53" s="25"/>
-      <c r="K53" s="25"/>
-      <c r="L53" s="25"/>
-      <c r="M53" s="25"/>
-      <c r="N53" s="25"/>
-      <c r="O53" s="26"/>
+      <c r="H53" s="25">
+        <v>1752.7460000000001</v>
+      </c>
+      <c r="I53" s="25">
+        <v>1999.9949999999999</v>
+      </c>
+      <c r="J53" s="25">
+        <v>1708.38</v>
+      </c>
+      <c r="K53" s="25">
+        <v>1548.596</v>
+      </c>
+      <c r="L53" s="25">
+        <v>1461.046</v>
+      </c>
+      <c r="M53" s="25">
+        <v>1413.076</v>
+      </c>
+      <c r="N53" s="25">
+        <v>1386.7909999999999</v>
+      </c>
+      <c r="O53" s="26">
+        <v>1372.3889999999999</v>
+      </c>
       <c r="P53" s="27">
         <f>SUM(C53:O53)</f>
-        <v>7195.12266</v>
+        <v>19838.141660000001</v>
       </c>
       <c r="Q53" s="30"/>
-      <c r="R53" s="30"/>
+      <c r="R53" s="120"/>
       <c r="S53" s="29"/>
       <c r="T53" s="29"/>
       <c r="U53" s="29"/>
@@ -3178,35 +3548,51 @@
       <c r="G54" s="72">
         <v>532.22735999999998</v>
       </c>
-      <c r="H54" s="34"/>
-      <c r="I54" s="34"/>
-      <c r="J54" s="34"/>
-      <c r="K54" s="34"/>
-      <c r="L54" s="34"/>
-      <c r="M54" s="34"/>
-      <c r="N54" s="34"/>
-      <c r="O54" s="35"/>
+      <c r="H54" s="34">
+        <v>768.60500000000002</v>
+      </c>
+      <c r="I54" s="34">
+        <v>875.649</v>
+      </c>
+      <c r="J54" s="34">
+        <v>749.45399999999995</v>
+      </c>
+      <c r="K54" s="34">
+        <v>680.30799999999999</v>
+      </c>
+      <c r="L54" s="34">
+        <v>642.42200000000003</v>
+      </c>
+      <c r="M54" s="34">
+        <v>621.66300000000001</v>
+      </c>
+      <c r="N54" s="34">
+        <v>610.28800000000001</v>
+      </c>
+      <c r="O54" s="35">
+        <v>604.05600000000004</v>
+      </c>
       <c r="P54" s="36">
-        <f t="shared" ref="P54:P58" si="12">SUM(C54:O54)</f>
-        <v>3163.1283599999988</v>
-      </c>
-      <c r="Q54" s="106">
+        <f t="shared" ref="P54:P58" si="13">SUM(C54:O54)</f>
+        <v>8715.5733600000003</v>
+      </c>
+      <c r="Q54" s="103">
         <v>1</v>
       </c>
-      <c r="R54" s="106">
+      <c r="R54" s="121">
         <v>2</v>
       </c>
-      <c r="S54" s="106">
+      <c r="S54" s="103">
         <v>3</v>
       </c>
-      <c r="T54" s="106">
+      <c r="T54" s="103">
         <v>4</v>
       </c>
-      <c r="U54" s="106">
+      <c r="U54" s="103">
         <v>5</v>
       </c>
       <c r="V54" s="29" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="55" spans="1:22" x14ac:dyDescent="0.25">
@@ -3232,36 +3618,52 @@
       <c r="G55" s="72">
         <v>368.65043999999989</v>
       </c>
-      <c r="H55" s="34"/>
-      <c r="I55" s="34"/>
-      <c r="J55" s="34"/>
-      <c r="K55" s="34"/>
-      <c r="L55" s="34"/>
-      <c r="M55" s="34"/>
-      <c r="N55" s="34"/>
-      <c r="O55" s="35"/>
+      <c r="H55" s="34">
+        <v>539.97400000000005</v>
+      </c>
+      <c r="I55" s="34">
+        <v>618.28499999999997</v>
+      </c>
+      <c r="J55" s="34">
+        <v>525.85400000000004</v>
+      </c>
+      <c r="K55" s="34">
+        <v>475.20699999999999</v>
+      </c>
+      <c r="L55" s="34">
+        <v>447.45800000000003</v>
+      </c>
+      <c r="M55" s="34">
+        <v>432.25299999999999</v>
+      </c>
+      <c r="N55" s="34">
+        <v>423.92099999999999</v>
+      </c>
+      <c r="O55" s="35">
+        <v>419.35599999999999</v>
+      </c>
       <c r="P55" s="36">
-        <f t="shared" si="12"/>
-        <v>2202.6704399999999</v>
+        <f t="shared" si="13"/>
+        <v>6084.9784399999999</v>
       </c>
       <c r="Q55" s="28">
         <f>C55/C$53</f>
         <v>0.30940988835725669</v>
       </c>
-      <c r="R55" s="28">
-        <f t="shared" ref="R55:U57" si="13">D55/D$53</f>
+      <c r="R55" s="122">
+        <f t="shared" ref="R55:U57" si="14">D55/D$53</f>
         <v>0.30515315961788586</v>
       </c>
       <c r="S55" s="28">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.30502392344497609</v>
       </c>
       <c r="T55" s="28">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.30494961798250464</v>
       </c>
       <c r="U55" s="28">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.30494961798250458</v>
       </c>
       <c r="V55" s="28">
@@ -3292,40 +3694,56 @@
       <c r="G56" s="72">
         <v>338.93351999999987</v>
       </c>
-      <c r="H56" s="34"/>
-      <c r="I56" s="34"/>
-      <c r="J56" s="34"/>
-      <c r="K56" s="34"/>
-      <c r="L56" s="34"/>
-      <c r="M56" s="34"/>
-      <c r="N56" s="34"/>
-      <c r="O56" s="35"/>
+      <c r="H56" s="34">
+        <v>507.23200000000003</v>
+      </c>
+      <c r="I56" s="34">
+        <v>585.25099999999998</v>
+      </c>
+      <c r="J56" s="34">
+        <v>493.05</v>
+      </c>
+      <c r="K56" s="34">
+        <v>442.53100000000001</v>
+      </c>
+      <c r="L56" s="34">
+        <v>414.85</v>
+      </c>
+      <c r="M56" s="34">
+        <v>399.68299999999999</v>
+      </c>
+      <c r="N56" s="34">
+        <v>391.37299999999999</v>
+      </c>
+      <c r="O56" s="35">
+        <v>386.81900000000002</v>
+      </c>
       <c r="P56" s="36">
-        <f t="shared" si="12"/>
-        <v>2039.6455199999996</v>
+        <f t="shared" si="13"/>
+        <v>5660.4345199999998</v>
       </c>
       <c r="Q56" s="28">
-        <f t="shared" ref="Q56:Q57" si="14">C56/C$53</f>
+        <f t="shared" ref="Q56:Q57" si="15">C56/C$53</f>
         <v>0.29277739804055586</v>
       </c>
-      <c r="R56" s="28">
-        <f t="shared" si="13"/>
+      <c r="R56" s="122">
+        <f t="shared" si="14"/>
         <v>0.28039646589227252</v>
       </c>
       <c r="S56" s="28">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.28020334928229662</v>
       </c>
       <c r="T56" s="28">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.2803676226331524</v>
       </c>
       <c r="U56" s="28">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.28036762263315235</v>
       </c>
       <c r="V56" s="28">
-        <f t="shared" ref="V56:V57" si="15">AVERAGE(Q56:U56)</f>
+        <f t="shared" ref="V56:V57" si="16">AVERAGE(Q56:U56)</f>
         <v>0.28282249169628593</v>
       </c>
     </row>
@@ -3352,40 +3770,56 @@
       <c r="G57" s="72">
         <v>954.89030999999989</v>
       </c>
-      <c r="H57" s="34"/>
-      <c r="I57" s="34"/>
-      <c r="J57" s="34"/>
-      <c r="K57" s="34"/>
-      <c r="L57" s="34"/>
-      <c r="M57" s="34"/>
-      <c r="N57" s="34"/>
-      <c r="O57" s="35"/>
+      <c r="H57" s="34">
+        <v>1412.742</v>
+      </c>
+      <c r="I57" s="34">
+        <v>1623.2760000000001</v>
+      </c>
+      <c r="J57" s="34">
+        <v>1374.6590000000001</v>
+      </c>
+      <c r="K57" s="34">
+        <v>1238.4349999999999</v>
+      </c>
+      <c r="L57" s="34">
+        <v>1163.7940000000001</v>
+      </c>
+      <c r="M57" s="34">
+        <v>1122.896</v>
+      </c>
+      <c r="N57" s="34">
+        <v>1100.4870000000001</v>
+      </c>
+      <c r="O57" s="35">
+        <v>1088.2090000000001</v>
+      </c>
       <c r="P57" s="36">
-        <f t="shared" si="12"/>
-        <v>5723.6873099999993</v>
+        <f t="shared" si="13"/>
+        <v>15848.185309999999</v>
       </c>
       <c r="Q57" s="28">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0.81161236424394312</v>
       </c>
-      <c r="R57" s="28">
+      <c r="R57" s="122">
         <f>D57/D$53</f>
         <v>0.79033053774050344</v>
       </c>
       <c r="S57" s="28">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.79002192982456143</v>
       </c>
       <c r="T57" s="28">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.78989037758830694</v>
       </c>
       <c r="U57" s="28">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.78989037758830682</v>
       </c>
       <c r="V57" s="28">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.79434911739712444</v>
       </c>
     </row>
@@ -3398,61 +3832,62 @@
         <v>31</v>
       </c>
       <c r="C58" s="39">
-        <f t="shared" ref="C58:O58" si="16">SUM(C53:C57)</f>
+        <f t="shared" ref="C58:O58" si="17">SUM(C53:C57)</f>
         <v>5180.5199999999995</v>
       </c>
       <c r="D58" s="39">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>4332.9239999999991</v>
       </c>
       <c r="E58" s="39">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>3898.3619999999996</v>
       </c>
       <c r="F58" s="39">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>3508.857</v>
       </c>
       <c r="G58" s="39">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>3403.5912899999998</v>
       </c>
       <c r="H58" s="39">
-        <f t="shared" si="16"/>
-        <v>0</v>
+        <f t="shared" si="17"/>
+        <v>4981.299</v>
       </c>
       <c r="I58" s="39">
-        <f t="shared" si="16"/>
-        <v>0</v>
+        <f t="shared" si="17"/>
+        <v>5702.4559999999992</v>
       </c>
       <c r="J58" s="39">
-        <f t="shared" si="16"/>
-        <v>0</v>
+        <f t="shared" si="17"/>
+        <v>4851.3970000000008</v>
       </c>
       <c r="K58" s="39">
-        <f t="shared" si="16"/>
-        <v>0</v>
+        <f t="shared" si="17"/>
+        <v>4385.0769999999993</v>
       </c>
       <c r="L58" s="39">
-        <f t="shared" si="16"/>
-        <v>0</v>
+        <f t="shared" si="17"/>
+        <v>4129.57</v>
       </c>
       <c r="M58" s="39">
-        <f t="shared" si="16"/>
-        <v>0</v>
+        <f t="shared" si="17"/>
+        <v>3989.5709999999999</v>
       </c>
       <c r="N58" s="39">
-        <f t="shared" si="16"/>
-        <v>0</v>
+        <f t="shared" si="17"/>
+        <v>3912.86</v>
       </c>
       <c r="O58" s="40">
-        <f t="shared" si="16"/>
-        <v>0</v>
+        <f t="shared" si="17"/>
+        <v>3870.8289999999997</v>
       </c>
       <c r="P58" s="41">
-        <f t="shared" si="12"/>
-        <v>20324.254290000001</v>
-      </c>
+        <f t="shared" si="13"/>
+        <v>56147.313289999991</v>
+      </c>
+      <c r="R58" s="123"/>
     </row>
     <row r="59" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A59" s="43"/>
@@ -3515,6 +3950,7 @@
         <v>7</v>
       </c>
       <c r="P60" s="95"/>
+      <c r="R60" s="124"/>
     </row>
     <row r="61" spans="1:22" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A61" s="43"/>
@@ -3561,9 +3997,13 @@
         <v>23</v>
       </c>
       <c r="P61" s="45"/>
-      <c r="Q61" s="21" t="s">
-        <v>45</v>
-      </c>
+      <c r="Q61" s="112" t="s">
+        <v>46</v>
+      </c>
+      <c r="R61" s="111"/>
+      <c r="S61" s="111"/>
+      <c r="T61" s="111"/>
+      <c r="U61" s="111"/>
       <c r="V61" s="28"/>
     </row>
     <row r="62" spans="1:22" s="51" customFormat="1" x14ac:dyDescent="0.25">
@@ -3616,6 +4056,7 @@
         <f>SUM(C62:O62)</f>
         <v>66645.686690430244</v>
       </c>
+      <c r="R62" s="125"/>
     </row>
     <row r="63" spans="1:22" s="57" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="52" t="s">
@@ -3636,23 +4077,23 @@
       <c r="N63" s="54"/>
       <c r="O63" s="55"/>
       <c r="P63" s="56"/>
-      <c r="Q63" s="107">
+      <c r="Q63" s="104">
         <v>1</v>
       </c>
-      <c r="R63" s="108">
+      <c r="R63" s="126">
         <v>2</v>
       </c>
-      <c r="S63" s="108">
+      <c r="S63" s="105">
         <v>3</v>
       </c>
-      <c r="T63" s="108">
+      <c r="T63" s="105">
         <v>4</v>
       </c>
-      <c r="U63" s="108">
+      <c r="U63" s="105">
         <v>5</v>
       </c>
-      <c r="V63" s="109" t="s">
-        <v>47</v>
+      <c r="V63" s="106" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="64" spans="1:22" s="57" customFormat="1" x14ac:dyDescent="0.25">
@@ -3676,20 +4117,20 @@
         <f>C55/C$54</f>
         <v>0.70759878419452893</v>
       </c>
-      <c r="R64" s="28">
-        <f t="shared" ref="R64:U66" si="17">D55/D$54</f>
+      <c r="R64" s="122">
+        <f t="shared" ref="R64:U66" si="18">D55/D$54</f>
         <v>0.69280114041340002</v>
       </c>
       <c r="S64" s="28">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0.69222938581608429</v>
       </c>
       <c r="T64" s="28">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0.69265593561368211</v>
       </c>
       <c r="U64" s="28">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0.69265593561368188</v>
       </c>
       <c r="V64" s="28">
@@ -3715,23 +4156,23 @@
       <c r="O65" s="62"/>
       <c r="P65" s="63"/>
       <c r="Q65" s="28">
-        <f t="shared" ref="Q65:Q66" si="18">C56/C$54</f>
+        <f t="shared" ref="Q65:Q66" si="19">C56/C$54</f>
         <v>0.66956144159791586</v>
       </c>
-      <c r="R65" s="28">
-        <f t="shared" si="17"/>
+      <c r="R65" s="122">
+        <f t="shared" si="18"/>
         <v>0.63659505142042572</v>
       </c>
       <c r="S65" s="28">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0.6359009161859519</v>
       </c>
       <c r="T65" s="28">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0.63682092555331993</v>
       </c>
       <c r="U65" s="28">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0.63682092555331971</v>
       </c>
       <c r="V65" s="28">
@@ -3757,23 +4198,23 @@
       <c r="O66" s="62"/>
       <c r="P66" s="63"/>
       <c r="Q66" s="28">
+        <f t="shared" si="19"/>
+        <v>1.8561007381676078</v>
+      </c>
+      <c r="R66" s="122">
         <f t="shared" si="18"/>
-        <v>1.8561007381676078</v>
-      </c>
-      <c r="R66" s="28">
-        <f t="shared" si="17"/>
         <v>1.794318297525711</v>
       </c>
       <c r="S66" s="28">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>1.7928967311390118</v>
       </c>
       <c r="T66" s="28">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>1.7941398390342056</v>
       </c>
       <c r="U66" s="28">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>1.7941398390342052</v>
       </c>
       <c r="V66" s="28">
@@ -3798,6 +4239,7 @@
       <c r="N67" s="66"/>
       <c r="O67" s="67"/>
       <c r="P67" s="68"/>
+      <c r="R67" s="127"/>
     </row>
     <row r="69" spans="1:22" s="16" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A69" s="13" t="s">
@@ -3846,6 +4288,7 @@
         <v>8</v>
       </c>
       <c r="P69"/>
+      <c r="R69" s="119"/>
     </row>
     <row r="70" spans="1:22" s="21" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A70" s="17" t="s">
@@ -3896,6 +4339,7 @@
       <c r="P70" s="20" t="s">
         <v>24</v>
       </c>
+      <c r="R70" s="128"/>
     </row>
     <row r="71" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A71" s="69" t="s">
@@ -3944,7 +4388,7 @@
       <c r="N72" s="34"/>
       <c r="O72" s="35"/>
       <c r="P72" s="36">
-        <f t="shared" ref="P72:P76" si="19">SUM(C72:O72)</f>
+        <f t="shared" ref="P72:P76" si="20">SUM(C72:O72)</f>
         <v>0</v>
       </c>
     </row>
@@ -3970,7 +4414,7 @@
       <c r="N73" s="34"/>
       <c r="O73" s="35"/>
       <c r="P73" s="36">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
     </row>
@@ -3996,7 +4440,7 @@
       <c r="N74" s="34"/>
       <c r="O74" s="35"/>
       <c r="P74" s="36">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
     </row>
@@ -4022,7 +4466,7 @@
       <c r="N75" s="34"/>
       <c r="O75" s="35"/>
       <c r="P75" s="36">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
     </row>
@@ -4035,59 +4479,59 @@
         <v>31</v>
       </c>
       <c r="C76" s="39">
-        <f t="shared" ref="C76:O76" si="20">SUM(C71:C75)</f>
+        <f t="shared" ref="C76:O76" si="21">SUM(C71:C75)</f>
         <v>0</v>
       </c>
       <c r="D76" s="39">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="E76" s="39">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="F76" s="39">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="G76" s="39">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="H76" s="39">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="I76" s="39">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="J76" s="39">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="K76" s="39">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="L76" s="39">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="M76" s="39">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="N76" s="39">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="O76" s="40">
+        <f t="shared" si="21"/>
+        <v>0</v>
+      </c>
+      <c r="P76" s="41">
         <f t="shared" si="20"/>
-        <v>0</v>
-      </c>
-      <c r="E76" s="39">
-        <f t="shared" si="20"/>
-        <v>0</v>
-      </c>
-      <c r="F76" s="39">
-        <f t="shared" si="20"/>
-        <v>0</v>
-      </c>
-      <c r="G76" s="39">
-        <f t="shared" si="20"/>
-        <v>0</v>
-      </c>
-      <c r="H76" s="39">
-        <f t="shared" si="20"/>
-        <v>0</v>
-      </c>
-      <c r="I76" s="39">
-        <f t="shared" si="20"/>
-        <v>0</v>
-      </c>
-      <c r="J76" s="39">
-        <f t="shared" si="20"/>
-        <v>0</v>
-      </c>
-      <c r="K76" s="39">
-        <f t="shared" si="20"/>
-        <v>0</v>
-      </c>
-      <c r="L76" s="39">
-        <f t="shared" si="20"/>
-        <v>0</v>
-      </c>
-      <c r="M76" s="39">
-        <f t="shared" si="20"/>
-        <v>0</v>
-      </c>
-      <c r="N76" s="39">
-        <f t="shared" si="20"/>
-        <v>0</v>
-      </c>
-      <c r="O76" s="40">
-        <f t="shared" si="20"/>
-        <v>0</v>
-      </c>
-      <c r="P76" s="41">
-        <f t="shared" si="19"/>
         <v>0</v>
       </c>
     </row>
@@ -4152,6 +4596,7 @@
         <v>7</v>
       </c>
       <c r="P78" s="95"/>
+      <c r="R78" s="124"/>
     </row>
     <row r="79" spans="1:22" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A79" s="43"/>
@@ -4250,7 +4695,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A81" s="52" t="s">
         <v>33</v>
       </c>
@@ -4270,7 +4715,7 @@
       <c r="O81" s="55"/>
       <c r="P81" s="56"/>
     </row>
-    <row r="82" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A82" s="61"/>
       <c r="B82" s="53"/>
       <c r="C82" s="54"/>
@@ -4288,7 +4733,7 @@
       <c r="O82" s="59"/>
       <c r="P82" s="60"/>
     </row>
-    <row r="83" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A83" s="61"/>
       <c r="B83" s="53"/>
       <c r="C83" s="53"/>
@@ -4306,7 +4751,7 @@
       <c r="O83" s="62"/>
       <c r="P83" s="63"/>
     </row>
-    <row r="84" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A84" s="61"/>
       <c r="B84" s="53"/>
       <c r="C84" s="53"/>
@@ -4324,7 +4769,7 @@
       <c r="O84" s="62"/>
       <c r="P84" s="63"/>
     </row>
-    <row r="85" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A85" s="65"/>
       <c r="B85" s="66"/>
       <c r="C85" s="66"/>
@@ -4342,7 +4787,7 @@
       <c r="O85" s="67"/>
       <c r="P85" s="68"/>
     </row>
-    <row r="87" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A87" s="79" t="s">
         <v>37</v>
       </c>
@@ -4350,63 +4795,63 @@
         <v>26</v>
       </c>
       <c r="C87" s="81">
-        <f t="shared" ref="C87:O87" si="21">C17+C35+C53+C71</f>
+        <f t="shared" ref="C87:O87" si="22">C17+C35+C53+C71</f>
         <v>6316.5690000000004</v>
       </c>
       <c r="D87" s="81">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>5348.2394999999997</v>
       </c>
       <c r="E87" s="81">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>4812.6239999999998</v>
       </c>
       <c r="F87" s="81">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>4332.4170000000004</v>
       </c>
       <c r="G87" s="81">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>4202.4444899999999</v>
       </c>
       <c r="H87" s="81">
-        <f t="shared" si="21"/>
-        <v>0</v>
+        <f t="shared" si="22"/>
+        <v>6469.0649999999996</v>
       </c>
       <c r="I87" s="81">
-        <f t="shared" si="21"/>
-        <v>0</v>
+        <f t="shared" si="22"/>
+        <v>6659.4129999999996</v>
       </c>
       <c r="J87" s="81">
-        <f t="shared" si="21"/>
-        <v>0</v>
+        <f t="shared" si="22"/>
+        <v>5822.3990000000003</v>
       </c>
       <c r="K87" s="81">
-        <f t="shared" si="21"/>
-        <v>0</v>
+        <f t="shared" si="22"/>
+        <v>5351.192</v>
       </c>
       <c r="L87" s="81">
-        <f t="shared" si="21"/>
-        <v>0</v>
+        <f t="shared" si="22"/>
+        <v>5085.3640000000005</v>
       </c>
       <c r="M87" s="81">
-        <f t="shared" si="21"/>
-        <v>0</v>
+        <f t="shared" si="22"/>
+        <v>4935.0709999999999</v>
       </c>
       <c r="N87" s="81">
-        <f t="shared" si="21"/>
-        <v>0</v>
+        <f t="shared" si="22"/>
+        <v>4849.9009999999998</v>
       </c>
       <c r="O87" s="82">
-        <f t="shared" si="21"/>
-        <v>0</v>
+        <f t="shared" si="22"/>
+        <v>4801.5240000000003</v>
       </c>
       <c r="P87" s="27">
         <f>SUM(C87:O87)</f>
-        <v>25012.293989999998</v>
-      </c>
-    </row>
-    <row r="88" spans="1:16" x14ac:dyDescent="0.25">
+        <v>68986.222989999995</v>
+      </c>
+    </row>
+    <row r="88" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A88" s="83" t="s">
         <v>37</v>
       </c>
@@ -4414,63 +4859,63 @@
         <v>27</v>
       </c>
       <c r="C88" s="85">
-        <f t="shared" ref="C88:O88" si="22">C18+C36+C54+C72</f>
+        <f t="shared" ref="C88:O88" si="23">C18+C36+C54+C72</f>
         <v>3659.3024999999998</v>
       </c>
       <c r="D88" s="85">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>3120.9734999999996</v>
       </c>
       <c r="E88" s="85">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>2809.5435000000002</v>
       </c>
       <c r="F88" s="85">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>2527.0320000000002</v>
       </c>
       <c r="G88" s="85">
-        <f t="shared" si="22"/>
+        <f t="shared" si="23"/>
         <v>2451.2210399999999</v>
       </c>
       <c r="H88" s="85">
-        <f t="shared" si="22"/>
-        <v>0</v>
+        <f t="shared" si="23"/>
+        <v>3792.6849999999999</v>
       </c>
       <c r="I88" s="85">
-        <f t="shared" si="22"/>
-        <v>0</v>
+        <f t="shared" si="23"/>
+        <v>3830.9019999999996</v>
       </c>
       <c r="J88" s="85">
-        <f t="shared" si="22"/>
-        <v>0</v>
+        <f t="shared" si="23"/>
+        <v>3370.55</v>
       </c>
       <c r="K88" s="85">
-        <f t="shared" si="22"/>
-        <v>0</v>
+        <f t="shared" si="23"/>
+        <v>3109.7860000000001</v>
       </c>
       <c r="L88" s="85">
-        <f t="shared" si="22"/>
-        <v>0</v>
+        <f t="shared" si="23"/>
+        <v>2961.73</v>
       </c>
       <c r="M88" s="85">
-        <f t="shared" si="22"/>
-        <v>0</v>
+        <f t="shared" si="23"/>
+        <v>2877.462</v>
       </c>
       <c r="N88" s="85">
-        <f t="shared" si="22"/>
-        <v>0</v>
+        <f t="shared" si="23"/>
+        <v>2829.3789999999999</v>
       </c>
       <c r="O88" s="86">
-        <f t="shared" si="22"/>
-        <v>0</v>
+        <f t="shared" si="23"/>
+        <v>2801.873</v>
       </c>
       <c r="P88" s="36">
-        <f t="shared" ref="P88:P92" si="23">SUM(C88:O88)</f>
-        <v>14568.072540000001</v>
-      </c>
-    </row>
-    <row r="89" spans="1:16" x14ac:dyDescent="0.25">
+        <f t="shared" ref="P88:P92" si="24">SUM(C88:O88)</f>
+        <v>40142.439539999999</v>
+      </c>
+    </row>
+    <row r="89" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A89" s="83" t="s">
         <v>37</v>
       </c>
@@ -4478,63 +4923,63 @@
         <v>38</v>
       </c>
       <c r="C89" s="85">
-        <f t="shared" ref="C89:O89" si="24">C19+C37+C55+C73</f>
+        <f t="shared" ref="C89:O89" si="25">C19+C37+C55+C73</f>
         <v>1885.6777737735356</v>
       </c>
       <c r="D89" s="85">
+        <f t="shared" si="25"/>
+        <v>1584.22326335463</v>
+      </c>
+      <c r="E89" s="85">
+        <f t="shared" si="25"/>
+        <v>1425.2751117224066</v>
+      </c>
+      <c r="F89" s="85">
+        <f t="shared" si="25"/>
+        <v>1282.6562522279246</v>
+      </c>
+      <c r="G89" s="85">
+        <f t="shared" si="25"/>
+        <v>1244.1765646610866</v>
+      </c>
+      <c r="H89" s="85">
+        <f t="shared" si="25"/>
+        <v>1924.1399999999999</v>
+      </c>
+      <c r="I89" s="85">
+        <f t="shared" si="25"/>
+        <v>1989.252</v>
+      </c>
+      <c r="J89" s="85">
+        <f t="shared" si="25"/>
+        <v>1733.8330000000001</v>
+      </c>
+      <c r="K89" s="85">
+        <f t="shared" si="25"/>
+        <v>1590.2109999999998</v>
+      </c>
+      <c r="L89" s="85">
+        <f t="shared" si="25"/>
+        <v>1509.2890000000002</v>
+      </c>
+      <c r="M89" s="85">
+        <f t="shared" si="25"/>
+        <v>1463.5959999999998</v>
+      </c>
+      <c r="N89" s="85">
+        <f t="shared" si="25"/>
+        <v>1437.7369999999999</v>
+      </c>
+      <c r="O89" s="86">
+        <f t="shared" si="25"/>
+        <v>1423.0700000000002</v>
+      </c>
+      <c r="P89" s="36">
         <f t="shared" si="24"/>
-        <v>1584.22326335463</v>
-      </c>
-      <c r="E89" s="85">
-        <f t="shared" si="24"/>
-        <v>1425.2751117224066</v>
-      </c>
-      <c r="F89" s="85">
-        <f t="shared" si="24"/>
-        <v>1282.6562522279246</v>
-      </c>
-      <c r="G89" s="85">
-        <f t="shared" si="24"/>
-        <v>1244.1765646610866</v>
-      </c>
-      <c r="H89" s="85">
-        <f t="shared" si="24"/>
-        <v>0</v>
-      </c>
-      <c r="I89" s="85">
-        <f t="shared" si="24"/>
-        <v>0</v>
-      </c>
-      <c r="J89" s="85">
-        <f t="shared" si="24"/>
-        <v>0</v>
-      </c>
-      <c r="K89" s="85">
-        <f t="shared" si="24"/>
-        <v>0</v>
-      </c>
-      <c r="L89" s="85">
-        <f t="shared" si="24"/>
-        <v>0</v>
-      </c>
-      <c r="M89" s="85">
-        <f t="shared" si="24"/>
-        <v>0</v>
-      </c>
-      <c r="N89" s="85">
-        <f t="shared" si="24"/>
-        <v>0</v>
-      </c>
-      <c r="O89" s="86">
-        <f t="shared" si="24"/>
-        <v>0</v>
-      </c>
-      <c r="P89" s="36">
-        <f t="shared" si="23"/>
-        <v>7422.0089657395838</v>
-      </c>
-    </row>
-    <row r="90" spans="1:16" x14ac:dyDescent="0.25">
+        <v>20493.136965739584</v>
+      </c>
+    </row>
+    <row r="90" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A90" s="83" t="s">
         <v>37</v>
       </c>
@@ -4542,63 +4987,63 @@
         <v>29</v>
       </c>
       <c r="C90" s="85">
-        <f t="shared" ref="C90:O90" si="25">C20+C38+C56+C74</f>
+        <f t="shared" ref="C90:O90" si="26">C20+C38+C56+C74</f>
         <v>2663.7221501511949</v>
       </c>
       <c r="D90" s="85">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>2192.9454003177016</v>
       </c>
       <c r="E90" s="85">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>1972.5442968624236</v>
       </c>
       <c r="F90" s="85">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>1776.1693240749757</v>
       </c>
       <c r="G90" s="85">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>1722.8842443527262</v>
       </c>
       <c r="H90" s="85">
-        <f t="shared" si="25"/>
-        <v>0</v>
+        <f t="shared" si="26"/>
+        <v>2767.777</v>
       </c>
       <c r="I90" s="85">
-        <f t="shared" si="25"/>
-        <v>0</v>
+        <f t="shared" si="26"/>
+        <v>2761.5529999999999</v>
       </c>
       <c r="J90" s="85">
-        <f t="shared" si="25"/>
-        <v>0</v>
+        <f t="shared" si="26"/>
+        <v>2413.87</v>
       </c>
       <c r="K90" s="85">
-        <f t="shared" si="25"/>
-        <v>0</v>
+        <f t="shared" si="26"/>
+        <v>2216.0929999999998</v>
       </c>
       <c r="L90" s="85">
-        <f t="shared" si="25"/>
-        <v>0</v>
+        <f t="shared" si="26"/>
+        <v>2103.3069999999998</v>
       </c>
       <c r="M90" s="85">
-        <f t="shared" si="25"/>
-        <v>0</v>
+        <f t="shared" si="26"/>
+        <v>2038.825</v>
       </c>
       <c r="N90" s="85">
-        <f t="shared" si="25"/>
-        <v>0</v>
+        <f t="shared" si="26"/>
+        <v>2001.8634999999999</v>
       </c>
       <c r="O90" s="86">
-        <f t="shared" si="25"/>
-        <v>0</v>
+        <f t="shared" si="26"/>
+        <v>1980.62</v>
       </c>
       <c r="P90" s="36">
-        <f t="shared" si="23"/>
-        <v>10328.265415759022</v>
-      </c>
-    </row>
-    <row r="91" spans="1:16" x14ac:dyDescent="0.25">
+        <f t="shared" si="24"/>
+        <v>28612.173915759024</v>
+      </c>
+    </row>
+    <row r="91" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A91" s="83" t="s">
         <v>37</v>
       </c>
@@ -4606,63 +5051,63 @@
         <v>30</v>
       </c>
       <c r="C91" s="85">
-        <f t="shared" ref="C91:O91" si="26">C21+C39+C57+C75</f>
+        <f t="shared" ref="C91:O91" si="27">C21+C39+C57+C75</f>
         <v>5155.3427990050513</v>
       </c>
       <c r="D91" s="85">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>4294.7260102158862</v>
       </c>
       <c r="E91" s="85">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>3863.9057938293527</v>
       </c>
       <c r="F91" s="85">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>3477.4472891239757</v>
       </c>
       <c r="G91" s="85">
-        <f t="shared" si="26"/>
+        <f t="shared" si="27"/>
         <v>3373.1238704502566</v>
       </c>
       <c r="H91" s="85">
-        <f t="shared" si="26"/>
-        <v>0</v>
+        <f t="shared" si="27"/>
+        <v>5272.0360000000001</v>
       </c>
       <c r="I91" s="85">
-        <f t="shared" si="26"/>
-        <v>0</v>
+        <f t="shared" si="27"/>
+        <v>5424.8019999999997</v>
       </c>
       <c r="J91" s="85">
-        <f t="shared" si="26"/>
-        <v>0</v>
+        <f t="shared" si="27"/>
+        <v>4722.0969999999998</v>
       </c>
       <c r="K91" s="85">
-        <f t="shared" si="26"/>
-        <v>0</v>
+        <f t="shared" si="27"/>
+        <v>4326.3379999999997</v>
       </c>
       <c r="L91" s="85">
-        <f t="shared" si="26"/>
-        <v>0</v>
+        <f t="shared" si="27"/>
+        <v>4102.9769999999999</v>
       </c>
       <c r="M91" s="85">
-        <f t="shared" si="26"/>
-        <v>0</v>
+        <f t="shared" si="27"/>
+        <v>3976.6350000000002</v>
       </c>
       <c r="N91" s="85">
-        <f t="shared" si="26"/>
-        <v>0</v>
+        <f t="shared" si="27"/>
+        <v>3905.0060000000003</v>
       </c>
       <c r="O91" s="86">
-        <f t="shared" si="26"/>
-        <v>0</v>
+        <f t="shared" si="27"/>
+        <v>3864.3</v>
       </c>
       <c r="P91" s="36">
-        <f t="shared" si="23"/>
-        <v>20164.545762624522</v>
-      </c>
-    </row>
-    <row r="92" spans="1:16" x14ac:dyDescent="0.25">
+        <f t="shared" si="24"/>
+        <v>55758.736762624525</v>
+      </c>
+    </row>
+    <row r="92" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A92" s="87" t="s">
         <v>39</v>
       </c>
@@ -4670,64 +5115,447 @@
         <v>31</v>
       </c>
       <c r="C92" s="89">
-        <f t="shared" ref="C92:O92" si="27">SUM(C87:C91)</f>
+        <f t="shared" ref="C92:O92" si="28">SUM(C87:C91)</f>
         <v>19680.614222929784</v>
       </c>
       <c r="D92" s="89">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>16541.107673888218</v>
       </c>
       <c r="E92" s="89">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>14883.892702414181</v>
       </c>
       <c r="F92" s="89">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>13395.721865426876</v>
       </c>
       <c r="G92" s="89">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>12993.850209464068</v>
       </c>
       <c r="H92" s="89">
-        <f t="shared" si="27"/>
-        <v>0</v>
+        <f t="shared" si="28"/>
+        <v>20225.703000000001</v>
       </c>
       <c r="I92" s="89">
-        <f t="shared" si="27"/>
-        <v>0</v>
+        <f t="shared" si="28"/>
+        <v>20665.921999999999</v>
       </c>
       <c r="J92" s="89">
-        <f t="shared" si="27"/>
-        <v>0</v>
+        <f t="shared" si="28"/>
+        <v>18062.749000000003</v>
       </c>
       <c r="K92" s="89">
-        <f t="shared" si="27"/>
-        <v>0</v>
+        <f t="shared" si="28"/>
+        <v>16593.62</v>
       </c>
       <c r="L92" s="89">
-        <f t="shared" si="27"/>
-        <v>0</v>
+        <f t="shared" si="28"/>
+        <v>15762.667000000001</v>
       </c>
       <c r="M92" s="89">
-        <f t="shared" si="27"/>
-        <v>0</v>
+        <f t="shared" si="28"/>
+        <v>15291.589</v>
       </c>
       <c r="N92" s="89">
-        <f t="shared" si="27"/>
-        <v>0</v>
+        <f t="shared" si="28"/>
+        <v>15023.886500000001</v>
       </c>
       <c r="O92" s="90">
-        <f t="shared" si="27"/>
-        <v>0</v>
+        <f t="shared" si="28"/>
+        <v>14871.386999999999</v>
       </c>
       <c r="P92" s="91">
-        <f t="shared" si="23"/>
-        <v>77495.186674123135</v>
+        <f t="shared" si="24"/>
+        <v>213992.71017412312</v>
+      </c>
+    </row>
+    <row r="96" spans="1:18" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="C96" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="D96" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="E96" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="F96" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="G96" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="H96" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="I96" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="J96" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="K96" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="L96" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="M96" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="N96" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="O96" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="P96" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="R96" s="129" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="97" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B97" t="s">
+        <v>52</v>
+      </c>
+      <c r="C97" s="48">
+        <v>5297.333333333333</v>
+      </c>
+      <c r="D97" s="48">
+        <v>4398.013245033113</v>
+      </c>
+      <c r="E97" s="48">
+        <v>4979.166666666667</v>
+      </c>
+      <c r="F97" s="48">
+        <v>13445</v>
+      </c>
+      <c r="G97" s="48">
+        <v>10433.32</v>
+      </c>
+      <c r="H97" s="48">
+        <v>9389.9879999999994</v>
+      </c>
+      <c r="I97" s="48">
+        <v>8920.4885999999988</v>
+      </c>
+      <c r="J97" s="48">
+        <v>8474.4641699999993</v>
+      </c>
+      <c r="K97" s="48">
+        <v>8050.7409614999988</v>
+      </c>
+      <c r="L97" s="48">
+        <v>7648.2039134249981</v>
+      </c>
+      <c r="M97" s="48">
+        <v>6597.0198675496695</v>
+      </c>
+      <c r="N97" s="48">
+        <v>6794.93046357616</v>
+      </c>
+      <c r="O97" s="49">
+        <v>6659.0318543046369</v>
+      </c>
+      <c r="P97" s="50">
+        <f>SUM(C97:O97)</f>
+        <v>101087.70107538856</v>
+      </c>
+      <c r="R97" s="130">
+        <v>127.59399999999999</v>
+      </c>
+    </row>
+    <row r="98" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B98" t="s">
+        <v>54</v>
+      </c>
+      <c r="C98" s="48">
+        <v>2375.2075</v>
+      </c>
+      <c r="D98" s="48">
+        <v>2171.5930769230768</v>
+      </c>
+      <c r="E98" s="48">
+        <v>2032.578</v>
+      </c>
+      <c r="F98" s="48">
+        <v>4572.9660000000003</v>
+      </c>
+      <c r="G98" s="48">
+        <v>5544.721274999999</v>
+      </c>
+      <c r="H98" s="48">
+        <v>4435.7770199999995</v>
+      </c>
+      <c r="I98" s="48">
+        <v>3548.6216159999999</v>
+      </c>
+      <c r="J98" s="48">
+        <v>3371.1905351999999</v>
+      </c>
+      <c r="K98" s="48">
+        <v>3202.6310084399997</v>
+      </c>
+      <c r="L98" s="48">
+        <v>3042.4994580179996</v>
+      </c>
+      <c r="M98" s="48">
+        <v>2981.6494688576395</v>
+      </c>
+      <c r="N98" s="48">
+        <v>3041.2824582347921</v>
+      </c>
+      <c r="O98" s="49">
+        <v>3071.6952828171402</v>
+      </c>
+      <c r="P98" s="50">
+        <f>SUM(C98:O98)</f>
+        <v>43392.412699490647</v>
+      </c>
+      <c r="R98" s="131">
+        <f>SUM(R101:R115)</f>
+        <v>1073.3809999999999</v>
+      </c>
+    </row>
+    <row r="99" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B99" t="s">
+        <v>53</v>
+      </c>
+      <c r="C99" s="48">
+        <v>3700.3714285714286</v>
+      </c>
+      <c r="D99" s="48">
+        <v>3333.0184615384605</v>
+      </c>
+      <c r="E99" s="48">
+        <v>3118.6895999999997</v>
+      </c>
+      <c r="F99" s="48">
+        <v>7017.7139999999999</v>
+      </c>
+      <c r="G99" s="48">
+        <v>8508.9782249999989</v>
+      </c>
+      <c r="H99" s="48">
+        <v>6807.1825799999997</v>
+      </c>
+      <c r="I99" s="48">
+        <v>5445.7460639999999</v>
+      </c>
+      <c r="J99" s="48">
+        <v>5173.4587607999993</v>
+      </c>
+      <c r="K99" s="48">
+        <v>4914.7858227599991</v>
+      </c>
+      <c r="L99" s="48">
+        <v>4669.0465316219988</v>
+      </c>
+      <c r="M99" s="48">
+        <v>4575.6656009895587</v>
+      </c>
+      <c r="N99" s="48">
+        <v>4667.1789130093503</v>
+      </c>
+      <c r="O99" s="49">
+        <v>4713.8507021394435</v>
+      </c>
+      <c r="P99" s="50">
+        <f>SUM(C99:O99)</f>
+        <v>66645.686690430244</v>
+      </c>
+      <c r="R99" s="130">
+        <v>4.3689999999999998</v>
+      </c>
+    </row>
+    <row r="101" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B101" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q101" s="115" t="s">
+        <v>57</v>
+      </c>
+      <c r="R101" s="116">
+        <v>30.178999999999998</v>
+      </c>
+    </row>
+    <row r="102" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B102" s="115" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q102" s="115" t="s">
+        <v>58</v>
+      </c>
+      <c r="R102" s="116">
+        <v>164.42500000000001</v>
+      </c>
+    </row>
+    <row r="103" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B103" s="115" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q103" s="115" t="s">
+        <v>59</v>
+      </c>
+      <c r="R103" s="116">
+        <v>0.70499999999999996</v>
+      </c>
+    </row>
+    <row r="104" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B104" s="115" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q104" s="115" t="s">
+        <v>60</v>
+      </c>
+      <c r="R104" s="116">
+        <v>0.41699999999999998</v>
+      </c>
+    </row>
+    <row r="105" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B105" s="115" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q105" s="115" t="s">
+        <v>61</v>
+      </c>
+      <c r="R105" s="116">
+        <v>14.289</v>
+      </c>
+    </row>
+    <row r="106" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B106" s="115" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q106" s="115" t="s">
+        <v>62</v>
+      </c>
+      <c r="R106" s="116">
+        <v>183.286</v>
+      </c>
+    </row>
+    <row r="107" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B107" s="115" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q107" s="115" t="s">
+        <v>63</v>
+      </c>
+      <c r="R107" s="116">
+        <v>237.64099999999999</v>
+      </c>
+    </row>
+    <row r="108" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B108" s="115" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q108" s="115" t="s">
+        <v>64</v>
+      </c>
+      <c r="R108" s="116">
+        <v>6.4370000000000003</v>
+      </c>
+    </row>
+    <row r="109" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B109" s="115" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q109" s="115" t="s">
+        <v>65</v>
+      </c>
+      <c r="R109" s="116">
+        <v>5.165</v>
+      </c>
+    </row>
+    <row r="110" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B110" s="115" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q110" s="115" t="s">
+        <v>66</v>
+      </c>
+      <c r="R110" s="116">
+        <v>28.251000000000001</v>
+      </c>
+    </row>
+    <row r="111" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B111" s="115" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q111" s="115" t="s">
+        <v>67</v>
+      </c>
+      <c r="R111" s="116">
+        <v>28.184999999999999</v>
+      </c>
+    </row>
+    <row r="112" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B112" s="115" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q112" s="115" t="s">
+        <v>68</v>
+      </c>
+      <c r="R112" s="116">
+        <v>171.73</v>
+      </c>
+    </row>
+    <row r="113" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B113" s="115" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q113" s="115" t="s">
+        <v>69</v>
+      </c>
+      <c r="R113" s="116">
+        <v>94.013000000000005</v>
+      </c>
+    </row>
+    <row r="114" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B114" s="115" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q114" s="115" t="s">
+        <v>70</v>
+      </c>
+      <c r="R114" s="116">
+        <v>20.401</v>
+      </c>
+    </row>
+    <row r="115" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B115" s="115" t="s">
+        <v>70</v>
+      </c>
+      <c r="Q115" s="115" t="s">
+        <v>71</v>
+      </c>
+      <c r="R115" s="116">
+        <v>88.257000000000005</v>
+      </c>
+    </row>
+    <row r="116" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B116" s="115" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="117" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B117" s="115" t="s">
+        <v>72</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="12">
+    <mergeCell ref="Q61:U61"/>
+    <mergeCell ref="X43:AB43"/>
+    <mergeCell ref="Q25:U25"/>
+    <mergeCell ref="Q16:U16"/>
+    <mergeCell ref="Q34:U34"/>
+    <mergeCell ref="Q43:U43"/>
+    <mergeCell ref="Q52:U52"/>
     <mergeCell ref="A1:P1"/>
     <mergeCell ref="B2:O2"/>
     <mergeCell ref="B3:O3"/>

</xml_diff>